<commit_message>
Modifications to the alphas and, probably, a modification in the method, using 3 differet alphas
</commit_message>
<xml_diff>
--- a/bip1271_data.xlsx
+++ b/bip1271_data.xlsx
@@ -14,12 +14,12 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="62">
   <si>
     <t>X</t>
   </si>
@@ -159,6 +159,18 @@
     <t>Nov-20</t>
   </si>
   <si>
+    <t xml:space="preserve">          croston_1271  SBA_1271  SBJ_1271 SES_bip1271</t>
+  </si>
+  <si>
+    <t>ME_1271       1.469275  2.490486  2.400955    4.079063</t>
+  </si>
+  <si>
+    <t>MAE_1271     12.256495 12.308866 12.142947   13.656211</t>
+  </si>
+  <si>
+    <t>RMSE_1271    15.799244 15.833640 15.732477   17.107302</t>
+  </si>
+  <si>
     <t>Forecast 1</t>
   </si>
   <si>
@@ -172,6 +184,27 @@
   </si>
   <si>
     <t>Forecast 5</t>
+  </si>
+  <si>
+    <t>croston_1271  SBA_1271  SBJ_1271 SES_bip1271</t>
+  </si>
+  <si>
+    <t>ME_1271       1.475555  1.813973  1.840646    5.552847</t>
+  </si>
+  <si>
+    <t>MAE_1271     12.059021 11.968242 11.962091   13.812953</t>
+  </si>
+  <si>
+    <t>RMSE_1271    15.583988 15.574060 15.575400   17.462432</t>
+  </si>
+  <si>
+    <t>ME_1271       1.135131  2.453853  2.605049    3.381521</t>
+  </si>
+  <si>
+    <t>MAE_1271     12.481392 12.079953 12.045239   13.695372</t>
+  </si>
+  <si>
+    <t>RMSE_1271    15.921076 15.945175 15.957732   16.969212</t>
   </si>
 </sst>
 </file>
@@ -2011,16 +2044,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>581024</xdr:colOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>609599</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>38099</xdr:rowOff>
+      <xdr:rowOff>123824</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>22</xdr:col>
-      <xdr:colOff>533400</xdr:colOff>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>561975</xdr:colOff>
       <xdr:row>29</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
+      <xdr:rowOff>142875</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2329,10 +2362,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J42"/>
+  <dimension ref="A1:S42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="X6" sqref="X6"/>
+      <selection activeCell="P45" sqref="P45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2838,7 +2871,7 @@
         <v>-13.76662073735792</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>25</v>
       </c>
@@ -2870,7 +2903,7 @@
         <v>24.298372373245769</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>26</v>
       </c>
@@ -2902,7 +2935,7 @@
         <v>27.6536165172589</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>27</v>
       </c>
@@ -2934,7 +2967,7 @@
         <v>-3.4944259603299308</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>28</v>
       </c>
@@ -2966,7 +2999,7 @@
         <v>-19.970262066280441</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>29</v>
       </c>
@@ -2998,7 +3031,7 @@
         <v>19.02527724366163</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>30</v>
       </c>
@@ -3030,7 +3063,7 @@
         <v>24.171485657112392</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>31</v>
       </c>
@@ -3062,7 +3095,7 @@
         <v>-12.454237191454469</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>32</v>
       </c>
@@ -3094,7 +3127,7 @@
         <v>-0.58610161273630013</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>33</v>
       </c>
@@ -3126,7 +3159,7 @@
         <v>-6.4981863708258558</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>34</v>
       </c>
@@ -3158,7 +3191,7 @@
         <v>-3.5234584152019761</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>35</v>
       </c>
@@ -3190,7 +3223,7 @@
         <v>6.0050603470783201</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>36</v>
       </c>
@@ -3222,7 +3255,7 @@
         <v>-7.8956987049834284</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>37</v>
       </c>
@@ -3254,7 +3287,7 @@
         <v>-16.71134389923591</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>38</v>
       </c>
@@ -3286,7 +3319,7 @@
         <v>-13.204642314350529</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>39</v>
       </c>
@@ -3318,7 +3351,7 @@
         <v>-10.223945967197951</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>40</v>
       </c>
@@ -3349,8 +3382,14 @@
       <c r="J32">
         <v>-13.690354072118261</v>
       </c>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L32" t="s">
+        <v>55</v>
+      </c>
+      <c r="S32" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="33" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>41</v>
       </c>
@@ -3381,8 +3420,14 @@
       <c r="J33">
         <v>15.363199038699481</v>
       </c>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L33" t="s">
+        <v>47</v>
+      </c>
+      <c r="S33" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="34" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>42</v>
       </c>
@@ -3413,8 +3458,14 @@
       <c r="J34">
         <v>-14.94128081710544</v>
       </c>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L34" t="s">
+        <v>48</v>
+      </c>
+      <c r="S34" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="35" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>43</v>
       </c>
@@ -3445,8 +3496,14 @@
       <c r="J35">
         <v>-12.70008869453962</v>
       </c>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L35" t="s">
+        <v>49</v>
+      </c>
+      <c r="S35" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="36" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>44</v>
       </c>
@@ -3478,7 +3535,7 @@
         <v>30.204924609641321</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>45</v>
       </c>
@@ -3510,9 +3567,9 @@
         <v>44.674185918195121</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="C38">
         <v>22.02694</v>
@@ -3526,10 +3583,13 @@
       <c r="F38">
         <v>21.985949999999999</v>
       </c>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="P38" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="39" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="C39">
         <v>22.02694</v>
@@ -3543,10 +3603,13 @@
       <c r="F39">
         <v>21.985949999999999</v>
       </c>
-    </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="P39" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="40" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="C40">
         <v>22.02694</v>
@@ -3560,10 +3623,13 @@
       <c r="F40">
         <v>21.985949999999999</v>
       </c>
-    </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="P40" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="41" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="C41">
         <v>22.02694</v>
@@ -3577,10 +3643,13 @@
       <c r="F41">
         <v>21.985949999999999</v>
       </c>
-    </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="P41" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="42" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="C42">
         <v>22.02694</v>

</xml_diff>

<commit_message>
Added errors and modified alphas of the first item. It will be evaluated according to 5 of them
</commit_message>
<xml_diff>
--- a/bip1271_data.xlsx
+++ b/bip1271_data.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="61">
   <si>
     <t>X</t>
   </si>
@@ -159,18 +159,6 @@
     <t>Nov-20</t>
   </si>
   <si>
-    <t xml:space="preserve">          croston_1271  SBA_1271  SBJ_1271 SES_bip1271</t>
-  </si>
-  <si>
-    <t>ME_1271       1.469275  2.490486  2.400955    4.079063</t>
-  </si>
-  <si>
-    <t>MAE_1271     12.256495 12.308866 12.142947   13.656211</t>
-  </si>
-  <si>
-    <t>RMSE_1271    15.799244 15.833640 15.732477   17.107302</t>
-  </si>
-  <si>
     <t>Forecast 1</t>
   </si>
   <si>
@@ -186,32 +174,44 @@
     <t>Forecast 5</t>
   </si>
   <si>
-    <t>croston_1271  SBA_1271  SBJ_1271 SES_bip1271</t>
-  </si>
-  <si>
-    <t>ME_1271       1.475555  1.813973  1.840646    5.552847</t>
-  </si>
-  <si>
-    <t>MAE_1271     12.059021 11.968242 11.962091   13.812953</t>
-  </si>
-  <si>
-    <t>RMSE_1271    15.583988 15.574060 15.575400   17.462432</t>
-  </si>
-  <si>
-    <t>ME_1271       1.135131  2.453853  2.605049    3.381521</t>
-  </si>
-  <si>
-    <t>MAE_1271     12.481392 12.079953 12.045239   13.695372</t>
-  </si>
-  <si>
-    <t>RMSE_1271    15.921076 15.945175 15.957732   16.969212</t>
+    <t>optimal</t>
+  </si>
+  <si>
+    <t>SES</t>
+  </si>
+  <si>
+    <t>Croston</t>
+  </si>
+  <si>
+    <t>SBA</t>
+  </si>
+  <si>
+    <t>SBJ</t>
+  </si>
+  <si>
+    <t>ME</t>
+  </si>
+  <si>
+    <t>MAE</t>
+  </si>
+  <si>
+    <t>RMSE</t>
+  </si>
+  <si>
+    <t>RMSE variation</t>
+  </si>
+  <si>
+    <t>MAE variation</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.000%"/>
+  </numFmts>
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -221,6 +221,13 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -245,17 +252,24 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -2362,10 +2376,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S42"/>
+  <dimension ref="A1:W67"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P45" sqref="P45"/>
+    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="O57" sqref="O57:S67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2375,6 +2389,7 @@
     <col min="5" max="5" width="14.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14" bestFit="1" customWidth="1"/>
     <col min="7" max="10" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2871,7 +2886,7 @@
         <v>-13.76662073735792</v>
       </c>
     </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>25</v>
       </c>
@@ -2903,7 +2918,7 @@
         <v>24.298372373245769</v>
       </c>
     </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>26</v>
       </c>
@@ -2935,7 +2950,7 @@
         <v>27.6536165172589</v>
       </c>
     </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>27</v>
       </c>
@@ -2967,7 +2982,7 @@
         <v>-3.4944259603299308</v>
       </c>
     </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>28</v>
       </c>
@@ -2999,7 +3014,7 @@
         <v>-19.970262066280441</v>
       </c>
     </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>29</v>
       </c>
@@ -3031,7 +3046,7 @@
         <v>19.02527724366163</v>
       </c>
     </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>30</v>
       </c>
@@ -3063,7 +3078,7 @@
         <v>24.171485657112392</v>
       </c>
     </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>31</v>
       </c>
@@ -3095,7 +3110,7 @@
         <v>-12.454237191454469</v>
       </c>
     </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>32</v>
       </c>
@@ -3127,7 +3142,7 @@
         <v>-0.58610161273630013</v>
       </c>
     </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>33</v>
       </c>
@@ -3159,7 +3174,7 @@
         <v>-6.4981863708258558</v>
       </c>
     </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>34</v>
       </c>
@@ -3191,7 +3206,7 @@
         <v>-3.5234584152019761</v>
       </c>
     </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>35</v>
       </c>
@@ -3223,7 +3238,7 @@
         <v>6.0050603470783201</v>
       </c>
     </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>36</v>
       </c>
@@ -3255,7 +3270,7 @@
         <v>-7.8956987049834284</v>
       </c>
     </row>
-    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>37</v>
       </c>
@@ -3287,7 +3302,7 @@
         <v>-16.71134389923591</v>
       </c>
     </row>
-    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>38</v>
       </c>
@@ -3319,7 +3334,7 @@
         <v>-13.204642314350529</v>
       </c>
     </row>
-    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>39</v>
       </c>
@@ -3351,7 +3366,7 @@
         <v>-10.223945967197951</v>
       </c>
     </row>
-    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>40</v>
       </c>
@@ -3382,14 +3397,14 @@
       <c r="J32">
         <v>-13.690354072118261</v>
       </c>
-      <c r="L32" t="s">
-        <v>55</v>
-      </c>
-      <c r="S32" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="33" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="N32">
+        <v>0.15</v>
+      </c>
+      <c r="T32">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>41</v>
       </c>
@@ -3420,14 +3435,32 @@
       <c r="J33">
         <v>15.363199038699481</v>
       </c>
-      <c r="L33" t="s">
-        <v>47</v>
-      </c>
-      <c r="S33" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="34" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="M33" t="s">
+        <v>52</v>
+      </c>
+      <c r="N33" t="s">
+        <v>53</v>
+      </c>
+      <c r="O33" t="s">
+        <v>54</v>
+      </c>
+      <c r="P33" t="s">
+        <v>55</v>
+      </c>
+      <c r="T33" t="s">
+        <v>52</v>
+      </c>
+      <c r="U33" t="s">
+        <v>53</v>
+      </c>
+      <c r="V33" t="s">
+        <v>54</v>
+      </c>
+      <c r="W33" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="34" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>42</v>
       </c>
@@ -3459,13 +3492,37 @@
         <v>-14.94128081710544</v>
       </c>
       <c r="L34" t="s">
-        <v>48</v>
+        <v>56</v>
+      </c>
+      <c r="M34" s="2">
+        <v>4.0790629999999997</v>
+      </c>
+      <c r="N34" s="2">
+        <v>1.4692750000000001</v>
+      </c>
+      <c r="O34" s="2">
+        <v>2.1390769999999999</v>
+      </c>
+      <c r="P34" s="2">
+        <v>2.1649449999999999</v>
       </c>
       <c r="S34" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="35" spans="1:19" x14ac:dyDescent="0.25">
+        <v>56</v>
+      </c>
+      <c r="T34" s="2">
+        <v>5.5528469999999999</v>
+      </c>
+      <c r="U34" s="2">
+        <v>1.4755549999999999</v>
+      </c>
+      <c r="V34" s="2">
+        <v>1.8139730000000001</v>
+      </c>
+      <c r="W34" s="2">
+        <v>1.840646</v>
+      </c>
+    </row>
+    <row r="35" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>43</v>
       </c>
@@ -3497,13 +3554,37 @@
         <v>-12.70008869453962</v>
       </c>
       <c r="L35" t="s">
-        <v>49</v>
+        <v>57</v>
+      </c>
+      <c r="M35" s="2">
+        <v>13.656211000000001</v>
+      </c>
+      <c r="N35" s="2">
+        <v>12.256494999999999</v>
+      </c>
+      <c r="O35" s="2">
+        <v>12.046198</v>
+      </c>
+      <c r="P35" s="2">
+        <v>12.036384</v>
       </c>
       <c r="S35" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="36" spans="1:19" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+      <c r="T35" s="2">
+        <v>13.812953</v>
+      </c>
+      <c r="U35" s="2">
+        <v>12.059021</v>
+      </c>
+      <c r="V35" s="2">
+        <v>11.968242</v>
+      </c>
+      <c r="W35" s="2">
+        <v>11.962090999999999</v>
+      </c>
+    </row>
+    <row r="36" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>44</v>
       </c>
@@ -3534,8 +3615,38 @@
       <c r="J36">
         <v>30.204924609641321</v>
       </c>
-    </row>
-    <row r="37" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="L36" t="s">
+        <v>58</v>
+      </c>
+      <c r="M36" s="2">
+        <v>17.107302000000001</v>
+      </c>
+      <c r="N36" s="2">
+        <v>15.799244</v>
+      </c>
+      <c r="O36" s="2">
+        <v>15.778325000000001</v>
+      </c>
+      <c r="P36" s="2">
+        <v>15.774134</v>
+      </c>
+      <c r="S36" t="s">
+        <v>58</v>
+      </c>
+      <c r="T36" s="2">
+        <v>17.462432</v>
+      </c>
+      <c r="U36" s="2">
+        <v>15.583988</v>
+      </c>
+      <c r="V36" s="2">
+        <v>15.574059999999999</v>
+      </c>
+      <c r="W36" s="2">
+        <v>15.5754</v>
+      </c>
+    </row>
+    <row r="37" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>45</v>
       </c>
@@ -3566,10 +3677,42 @@
       <c r="J37">
         <v>44.674185918195121</v>
       </c>
-    </row>
-    <row r="38" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="L37" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="M37" s="4"/>
+      <c r="N37" s="4">
+        <f>(M36-N36)/N36</f>
+        <v>8.2792442473829816E-2</v>
+      </c>
+      <c r="O37" s="4">
+        <f>(M36-O36)/O36</f>
+        <v>8.422801533115841E-2</v>
+      </c>
+      <c r="P37" s="4">
+        <f>(M36-P36)/P36</f>
+        <v>8.4516081833715909E-2</v>
+      </c>
+      <c r="S37" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="T37" s="4"/>
+      <c r="U37" s="4">
+        <f>(T36-U36)/U36</f>
+        <v>0.12053679712792387</v>
+      </c>
+      <c r="V37" s="4">
+        <f>(T36-V36)/V36</f>
+        <v>0.12125110600575575</v>
+      </c>
+      <c r="W37" s="4">
+        <f>(T36-W36)/W36</f>
+        <v>0.1211546412933215</v>
+      </c>
+    </row>
+    <row r="38" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="C38">
         <v>22.02694</v>
@@ -3583,13 +3726,32 @@
       <c r="F38">
         <v>21.985949999999999</v>
       </c>
-      <c r="P38" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="39" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="L38" s="3"/>
+      <c r="M38" s="4"/>
+      <c r="N38" s="4"/>
+      <c r="O38" s="4">
+        <f>(N36-O36)/O36</f>
+        <v>1.3258061296113018E-3</v>
+      </c>
+      <c r="P38" s="4">
+        <f>(N36-P36)/P36</f>
+        <v>1.5918465000994504E-3</v>
+      </c>
+      <c r="S38" s="3"/>
+      <c r="T38" s="4"/>
+      <c r="U38" s="4"/>
+      <c r="V38" s="4">
+        <f>($U$36-V36)/V36</f>
+        <v>6.3747025502665215E-4</v>
+      </c>
+      <c r="W38" s="4">
+        <f>($U$36-W36)/W36</f>
+        <v>5.5138230799848457E-4</v>
+      </c>
+    </row>
+    <row r="39" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="C39">
         <v>22.02694</v>
@@ -3603,13 +3765,26 @@
       <c r="F39">
         <v>21.985949999999999</v>
       </c>
-      <c r="P39" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="40" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="L39" s="3"/>
+      <c r="M39" s="4"/>
+      <c r="N39" s="4"/>
+      <c r="O39" s="4"/>
+      <c r="P39" s="4">
+        <f>(O36-P36)/P36</f>
+        <v>2.6568811955068341E-4</v>
+      </c>
+      <c r="S39" s="3"/>
+      <c r="T39" s="4"/>
+      <c r="U39" s="4"/>
+      <c r="V39" s="4"/>
+      <c r="W39" s="4">
+        <f>($V$36-W36)/W36</f>
+        <v>-8.6033103483749057E-5</v>
+      </c>
+    </row>
+    <row r="40" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="C40">
         <v>22.02694</v>
@@ -3623,13 +3798,40 @@
       <c r="F40">
         <v>21.985949999999999</v>
       </c>
-      <c r="P40" t="s">
+      <c r="L40" s="3" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="41" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="N40" s="4">
+        <f>(M35-N35)/N35</f>
+        <v>0.11420198025618267</v>
+      </c>
+      <c r="O40" s="4">
+        <f>(M35-O35)/O35</f>
+        <v>0.13365320742694087</v>
+      </c>
+      <c r="P40" s="4">
+        <f>(M35-P35)/P35</f>
+        <v>0.1345775442192606</v>
+      </c>
+      <c r="S40" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="U40" s="4">
+        <f>($T$35-U35)/U35</f>
+        <v>0.14544563775119065</v>
+      </c>
+      <c r="V40" s="4">
+        <f t="shared" ref="V40:W40" si="0">($T$35-V35)/V35</f>
+        <v>0.15413383185266477</v>
+      </c>
+      <c r="W40" s="4">
+        <f t="shared" si="0"/>
+        <v>0.15472729642334282</v>
+      </c>
+    </row>
+    <row r="41" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="C41">
         <v>22.02694</v>
@@ -3643,13 +3845,28 @@
       <c r="F41">
         <v>21.985949999999999</v>
       </c>
-      <c r="P41" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="42" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="L41" s="3"/>
+      <c r="O41" s="4">
+        <f>(N35-O35)/O35</f>
+        <v>1.7457541375295246E-2</v>
+      </c>
+      <c r="P41" s="4">
+        <f>(N35-P35)/P35</f>
+        <v>1.82871367347535E-2</v>
+      </c>
+      <c r="S41" s="3"/>
+      <c r="V41" s="4">
+        <f>($U$35-V35)/V35</f>
+        <v>7.584990343610991E-3</v>
+      </c>
+      <c r="W41" s="4">
+        <f>($U$35-W35)/W35</f>
+        <v>8.1030983629869074E-3</v>
+      </c>
+    </row>
+    <row r="42" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="C42">
         <v>22.02694</v>
@@ -3663,8 +3880,460 @@
       <c r="F42">
         <v>21.985949999999999</v>
       </c>
+      <c r="L42" s="3"/>
+      <c r="P42" s="4">
+        <f>(O35-P35)/P35</f>
+        <v>8.1536115830139956E-4</v>
+      </c>
+      <c r="S42" s="3"/>
+      <c r="W42" s="4">
+        <f>($V$35-W35)/W35</f>
+        <v>5.1420775849313519E-4</v>
+      </c>
+    </row>
+    <row r="44" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="N44">
+        <v>0.2</v>
+      </c>
+      <c r="U44">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="45" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="M45" t="s">
+        <v>52</v>
+      </c>
+      <c r="N45" t="s">
+        <v>53</v>
+      </c>
+      <c r="O45" t="s">
+        <v>54</v>
+      </c>
+      <c r="P45" t="s">
+        <v>55</v>
+      </c>
+      <c r="T45" t="s">
+        <v>52</v>
+      </c>
+      <c r="U45" t="s">
+        <v>53</v>
+      </c>
+      <c r="V45" t="s">
+        <v>54</v>
+      </c>
+      <c r="W45" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="46" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="L46" t="s">
+        <v>56</v>
+      </c>
+      <c r="M46" s="2">
+        <v>3.3815210000000002</v>
+      </c>
+      <c r="N46" s="2">
+        <v>1.1351309999999999</v>
+      </c>
+      <c r="O46" s="2">
+        <v>2.4538530000000001</v>
+      </c>
+      <c r="P46" s="2">
+        <v>2.6050490000000002</v>
+      </c>
+      <c r="S46" t="s">
+        <v>56</v>
+      </c>
+      <c r="T46" s="2">
+        <v>1.7806340000000001</v>
+      </c>
+      <c r="U46" s="2">
+        <v>0.54734760000000005</v>
+      </c>
+      <c r="V46" s="2">
+        <v>8.4957940000000001</v>
+      </c>
+      <c r="W46" s="2">
+        <v>15.22409</v>
+      </c>
+    </row>
+    <row r="47" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="L47" t="s">
+        <v>57</v>
+      </c>
+      <c r="M47" s="2">
+        <v>13.695372000000001</v>
+      </c>
+      <c r="N47" s="2">
+        <v>12.481392</v>
+      </c>
+      <c r="O47" s="2">
+        <v>12.079953</v>
+      </c>
+      <c r="P47" s="2">
+        <v>12.045239</v>
+      </c>
+      <c r="S47" t="s">
+        <v>57</v>
+      </c>
+      <c r="T47" s="2">
+        <v>13.537411000000001</v>
+      </c>
+      <c r="U47" s="2">
+        <v>13.6922487</v>
+      </c>
+      <c r="V47" s="2">
+        <v>12.758718999999999</v>
+      </c>
+      <c r="W47" s="2">
+        <v>15.892720000000001</v>
+      </c>
+    </row>
+    <row r="48" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="L48" t="s">
+        <v>58</v>
+      </c>
+      <c r="M48" s="2">
+        <v>16.969211999999999</v>
+      </c>
+      <c r="N48" s="2">
+        <v>15.921075999999999</v>
+      </c>
+      <c r="O48" s="2">
+        <v>15.945175000000001</v>
+      </c>
+      <c r="P48" s="2">
+        <v>15.957732</v>
+      </c>
+      <c r="S48" t="s">
+        <v>58</v>
+      </c>
+      <c r="T48" s="2">
+        <v>17.427333000000001</v>
+      </c>
+      <c r="U48" s="2">
+        <v>17.939190199999999</v>
+      </c>
+      <c r="V48" s="2">
+        <v>18.078852000000001</v>
+      </c>
+      <c r="W48" s="2">
+        <v>21.77338</v>
+      </c>
+    </row>
+    <row r="49" spans="12:23" x14ac:dyDescent="0.25">
+      <c r="L49" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="M49" s="4"/>
+      <c r="N49" s="4">
+        <f>(M48-N48)/N48</f>
+        <v>6.5833238909229472E-2</v>
+      </c>
+      <c r="O49" s="4">
+        <f>(M48-O48)/O48</f>
+        <v>6.422237448005419E-2</v>
+      </c>
+      <c r="P49" s="4">
+        <f>(M48-P48)/P48</f>
+        <v>6.3384947184223855E-2</v>
+      </c>
+      <c r="S49" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="T49" s="4"/>
+      <c r="U49" s="4">
+        <f>(T48-U48)/U48</f>
+        <v>-2.8532904456300259E-2</v>
+      </c>
+      <c r="V49" s="4">
+        <f>(T48-V48)/V48</f>
+        <v>-3.6037631150473509E-2</v>
+      </c>
+      <c r="W49" s="4">
+        <f>(T48-W48)/W48</f>
+        <v>-0.19960369037788339</v>
+      </c>
+    </row>
+    <row r="50" spans="12:23" x14ac:dyDescent="0.25">
+      <c r="L50" s="3"/>
+      <c r="M50" s="4"/>
+      <c r="N50" s="4"/>
+      <c r="O50" s="4">
+        <f>(N48-O48)/O48</f>
+        <v>-1.5113662910567884E-3</v>
+      </c>
+      <c r="P50" s="4">
+        <f>(N48-P48)/P48</f>
+        <v>-2.2970682801290738E-3</v>
+      </c>
+      <c r="S50" s="3"/>
+      <c r="T50" s="4"/>
+      <c r="U50" s="4"/>
+      <c r="V50" s="4">
+        <f>(U48-V48)/V48</f>
+        <v>-7.7251475923362E-3</v>
+      </c>
+      <c r="W50" s="4">
+        <f>(U48-W48)/W48</f>
+        <v>-0.17609529618277001</v>
+      </c>
+    </row>
+    <row r="51" spans="12:23" x14ac:dyDescent="0.25">
+      <c r="L51" s="3"/>
+      <c r="M51" s="4"/>
+      <c r="N51" s="4"/>
+      <c r="O51" s="4"/>
+      <c r="P51" s="4">
+        <f>(O48-P48)/P48</f>
+        <v>-7.8689127001250949E-4</v>
+      </c>
+      <c r="S51" s="3"/>
+      <c r="T51" s="4"/>
+      <c r="U51" s="4"/>
+      <c r="V51" s="4"/>
+      <c r="W51" s="4">
+        <f>(V48-W48)/W48</f>
+        <v>-0.16968095904264741</v>
+      </c>
+    </row>
+    <row r="52" spans="12:23" x14ac:dyDescent="0.25">
+      <c r="L52" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="N52" s="4">
+        <f>(M47-N47)/N47</f>
+        <v>9.7263189874975578E-2</v>
+      </c>
+      <c r="O52" s="4">
+        <f>(M47-O47)/O47</f>
+        <v>0.13372725870704968</v>
+      </c>
+      <c r="P52" s="4">
+        <f>(M47-P47)/P47</f>
+        <v>0.13699462501325213</v>
+      </c>
+      <c r="S52" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="U52" s="4">
+        <f>(T47-U47)/U47</f>
+        <v>-1.1308420069816571E-2</v>
+      </c>
+      <c r="V52" s="4">
+        <f>(T47-V47)/V47</f>
+        <v>6.1032145938789098E-2</v>
+      </c>
+      <c r="W52" s="4">
+        <f>(T47-W47)/W47</f>
+        <v>-0.14820049683125355</v>
+      </c>
+    </row>
+    <row r="53" spans="12:23" x14ac:dyDescent="0.25">
+      <c r="L53" s="3"/>
+      <c r="O53" s="4">
+        <f>(N47-O47)/O47</f>
+        <v>3.3231834594058429E-2</v>
+      </c>
+      <c r="P53" s="4">
+        <f>(N47-P47)/P47</f>
+        <v>3.6209576248341695E-2</v>
+      </c>
+      <c r="S53" s="3"/>
+      <c r="V53" s="4">
+        <f>(U47-V47)/V47</f>
+        <v>7.3167980265103516E-2</v>
+      </c>
+      <c r="W53" s="4">
+        <f>(U47-W47)/W47</f>
+        <v>-0.13845781590564737</v>
+      </c>
+    </row>
+    <row r="54" spans="12:23" x14ac:dyDescent="0.25">
+      <c r="L54" s="3"/>
+      <c r="P54" s="4">
+        <f>(O47-P47)/P47</f>
+        <v>2.8819685520560649E-3</v>
+      </c>
+      <c r="S54" s="3"/>
+      <c r="W54" s="4">
+        <f>(V47-W47)/W47</f>
+        <v>-0.19719727019666874</v>
+      </c>
+    </row>
+    <row r="56" spans="12:23" x14ac:dyDescent="0.25">
+      <c r="Q56" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="57" spans="12:23" x14ac:dyDescent="0.25">
+      <c r="P57">
+        <v>0.32479999999999998</v>
+      </c>
+      <c r="Q57">
+        <v>9.7500000000000003E-2</v>
+      </c>
+      <c r="R57">
+        <v>8.3199999999999996E-2</v>
+      </c>
+      <c r="S57">
+        <v>9.1399999999999995E-2</v>
+      </c>
+    </row>
+    <row r="58" spans="12:23" x14ac:dyDescent="0.25">
+      <c r="P58" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q58" t="s">
+        <v>53</v>
+      </c>
+      <c r="R58" t="s">
+        <v>54</v>
+      </c>
+      <c r="S58" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="59" spans="12:23" x14ac:dyDescent="0.25">
+      <c r="O59" t="s">
+        <v>56</v>
+      </c>
+      <c r="P59" s="2">
+        <v>2.6796150000000001</v>
+      </c>
+      <c r="Q59" s="2">
+        <v>2.4482569999999999</v>
+      </c>
+      <c r="R59" s="2">
+        <v>2.4904860000000002</v>
+      </c>
+      <c r="S59" s="2">
+        <v>2.4009550000000002</v>
+      </c>
+    </row>
+    <row r="60" spans="12:23" x14ac:dyDescent="0.25">
+      <c r="O60" t="s">
+        <v>57</v>
+      </c>
+      <c r="P60" s="2">
+        <v>13.580219</v>
+      </c>
+      <c r="Q60" s="2">
+        <v>12.237493000000001</v>
+      </c>
+      <c r="R60" s="2">
+        <v>12.308866</v>
+      </c>
+      <c r="S60" s="2">
+        <v>12.142946999999999</v>
+      </c>
+    </row>
+    <row r="61" spans="12:23" x14ac:dyDescent="0.25">
+      <c r="O61" t="s">
+        <v>58</v>
+      </c>
+      <c r="P61" s="2">
+        <v>16.884156999999998</v>
+      </c>
+      <c r="Q61" s="2">
+        <v>15.788823000000001</v>
+      </c>
+      <c r="R61" s="2">
+        <v>15.833640000000001</v>
+      </c>
+      <c r="S61" s="2">
+        <v>15.732476999999999</v>
+      </c>
+    </row>
+    <row r="62" spans="12:23" x14ac:dyDescent="0.25">
+      <c r="O62" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="P62" s="4"/>
+      <c r="Q62" s="4">
+        <f>(P61-Q61)/Q61</f>
+        <v>6.9374012236377444E-2</v>
+      </c>
+      <c r="R62" s="4">
+        <f>(P61-R61)/R61</f>
+        <v>6.6347157065589302E-2</v>
+      </c>
+      <c r="S62" s="4">
+        <f>(P61-S61)/S61</f>
+        <v>7.3203984343978318E-2</v>
+      </c>
+    </row>
+    <row r="63" spans="12:23" x14ac:dyDescent="0.25">
+      <c r="O63" s="3"/>
+      <c r="P63" s="4"/>
+      <c r="Q63" s="4"/>
+      <c r="R63" s="4">
+        <f>(Q61-R61)/R61</f>
+        <v>-2.8304925462496371E-3</v>
+      </c>
+      <c r="S63" s="4">
+        <f>(Q61-S61)/S61</f>
+        <v>3.5815084935449989E-3</v>
+      </c>
+    </row>
+    <row r="64" spans="12:23" x14ac:dyDescent="0.25">
+      <c r="O64" s="3"/>
+      <c r="P64" s="4"/>
+      <c r="Q64" s="4"/>
+      <c r="R64" s="4"/>
+      <c r="S64" s="4">
+        <f>(R61-S61)/S61</f>
+        <v>6.4302016777142883E-3</v>
+      </c>
+    </row>
+    <row r="65" spans="15:19" x14ac:dyDescent="0.25">
+      <c r="O65" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="Q65" s="4">
+        <f>(P60-Q60)/Q60</f>
+        <v>0.10972230995351735</v>
+      </c>
+      <c r="R65" s="4">
+        <f>(P60-R60)/R60</f>
+        <v>0.10328758148801032</v>
+      </c>
+      <c r="S65" s="4">
+        <f>(P60-S60)/S60</f>
+        <v>0.11836270058660391</v>
+      </c>
+    </row>
+    <row r="66" spans="15:19" x14ac:dyDescent="0.25">
+      <c r="O66" s="3"/>
+      <c r="R66" s="4">
+        <f>(Q60-R60)/R60</f>
+        <v>-5.7985032902299416E-3</v>
+      </c>
+      <c r="S66" s="4">
+        <f>(Q60-S60)/S60</f>
+        <v>7.7860835594523413E-3</v>
+      </c>
+    </row>
+    <row r="67" spans="15:19" x14ac:dyDescent="0.25">
+      <c r="O67" s="3"/>
+      <c r="S67" s="4">
+        <f>(R60-S60)/S60</f>
+        <v>1.3663816534816514E-2</v>
+      </c>
     </row>
   </sheetData>
+  <mergeCells count="10">
+    <mergeCell ref="O62:O64"/>
+    <mergeCell ref="O65:O67"/>
+    <mergeCell ref="S37:S39"/>
+    <mergeCell ref="S40:S42"/>
+    <mergeCell ref="L37:L39"/>
+    <mergeCell ref="L40:L42"/>
+    <mergeCell ref="L49:L51"/>
+    <mergeCell ref="L52:L54"/>
+    <mergeCell ref="S49:S51"/>
+    <mergeCell ref="S52:S54"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>

</xml_diff>

<commit_message>
Modifications to the the main results data
</commit_message>
<xml_diff>
--- a/bip1271_data.xlsx
+++ b/bip1271_data.xlsx
@@ -26,11 +26,12 @@
     <externalReference r:id="rId10"/>
   </externalReferences>
   <calcPr calcId="162913"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="379" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="66">
   <si>
     <t>X</t>
   </si>
@@ -218,10 +219,16 @@
     <t>SES_bip1271.1</t>
   </si>
   <si>
-    <t>NA</t>
+    <t>opt</t>
   </si>
   <si>
-    <t>opt</t>
+    <t>Cro.</t>
+  </si>
+  <si>
+    <t>yt</t>
+  </si>
+  <si>
+    <t>t</t>
   </si>
 </sst>
 </file>
@@ -255,12 +262,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -276,28 +289,29 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -356,7 +370,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1476,7 +1489,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1588,7 +1600,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3186,7 +3197,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3298,7 +3308,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4896,7 +4905,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -5008,7 +5016,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -6546,7 +6553,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -6743,7 +6749,7 @@
             <c:strRef>
               <c:f>[4]Sheet1!$A$2:$A$42</c:f>
               <c:strCache>
-                <c:ptCount val="36"/>
+                <c:ptCount val="41"/>
                 <c:pt idx="0">
                   <c:v>Dec-17</c:v>
                 </c:pt>
@@ -7021,7 +7027,7 @@
             <c:strRef>
               <c:f>[4]Sheet1!$A$2:$A$42</c:f>
               <c:strCache>
-                <c:ptCount val="36"/>
+                <c:ptCount val="41"/>
                 <c:pt idx="0">
                   <c:v>Dec-17</c:v>
                 </c:pt>
@@ -7314,7 +7320,7 @@
             <c:strRef>
               <c:f>[4]Sheet1!$A$2:$A$42</c:f>
               <c:strCache>
-                <c:ptCount val="36"/>
+                <c:ptCount val="41"/>
                 <c:pt idx="0">
                   <c:v>Dec-17</c:v>
                 </c:pt>
@@ -7601,7 +7607,7 @@
             <c:strRef>
               <c:f>[4]Sheet1!$A$2:$A$42</c:f>
               <c:strCache>
-                <c:ptCount val="36"/>
+                <c:ptCount val="41"/>
                 <c:pt idx="0">
                   <c:v>Dec-17</c:v>
                 </c:pt>
@@ -7888,7 +7894,7 @@
             <c:strRef>
               <c:f>[4]Sheet1!$A$2:$A$42</c:f>
               <c:strCache>
-                <c:ptCount val="36"/>
+                <c:ptCount val="41"/>
                 <c:pt idx="0">
                   <c:v>Dec-17</c:v>
                 </c:pt>
@@ -8263,7 +8269,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -16015,20 +16020,20 @@
       <c r="F38">
         <v>21.985949999999999</v>
       </c>
-      <c r="L38" s="4" t="s">
+      <c r="L38" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="M38" s="4"/>
-      <c r="N38" s="4"/>
-      <c r="O38" s="4"/>
-      <c r="P38" s="4"/>
-      <c r="S38" s="4" t="s">
+      <c r="M38" s="8"/>
+      <c r="N38" s="8"/>
+      <c r="O38" s="8"/>
+      <c r="P38" s="8"/>
+      <c r="S38" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="T38" s="4"/>
-      <c r="U38" s="4"/>
-      <c r="V38" s="4"/>
-      <c r="W38" s="4"/>
+      <c r="T38" s="8"/>
+      <c r="U38" s="8"/>
+      <c r="V38" s="8"/>
+      <c r="W38" s="8"/>
     </row>
     <row r="39" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
@@ -16046,35 +16051,35 @@
       <c r="F39">
         <v>21.985949999999999</v>
       </c>
-      <c r="L39" s="5" t="s">
+      <c r="L39" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="M39" s="6"/>
-      <c r="N39" s="6">
+      <c r="M39" s="5"/>
+      <c r="N39" s="5">
         <f>(M36-N36)/N36</f>
         <v>0.12053679712792387</v>
       </c>
-      <c r="O39" s="6">
+      <c r="O39" s="5">
         <f>(M36-O36)/O36</f>
         <v>0.12125110600575575</v>
       </c>
-      <c r="P39" s="6">
+      <c r="P39" s="5">
         <f>(M36-P36)/P36</f>
         <v>0.1211546412933215</v>
       </c>
-      <c r="S39" s="5" t="s">
+      <c r="S39" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="T39" s="6"/>
-      <c r="U39" s="6">
+      <c r="T39" s="5"/>
+      <c r="U39" s="5">
         <f>(T36-U36)/U36</f>
         <v>8.2792442473829816E-2</v>
       </c>
-      <c r="V39" s="6">
+      <c r="V39" s="5">
         <f>(T36-V36)/V36</f>
         <v>8.422801533115841E-2</v>
       </c>
-      <c r="W39" s="6">
+      <c r="W39" s="5">
         <f>(T36-W36)/W36</f>
         <v>8.4516081833715909E-2</v>
       </c>
@@ -16095,35 +16100,35 @@
       <c r="F40">
         <v>21.985949999999999</v>
       </c>
-      <c r="L40" s="5" t="s">
+      <c r="L40" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="M40" s="6">
+      <c r="M40" s="5">
         <f>(N36-M36)/M36</f>
         <v>-0.10757058352467744</v>
       </c>
-      <c r="N40" s="6"/>
-      <c r="O40" s="6">
+      <c r="N40" s="5"/>
+      <c r="O40" s="5">
         <f>(N36-O36)/O36</f>
         <v>6.3747025502665215E-4</v>
       </c>
-      <c r="P40" s="6">
+      <c r="P40" s="5">
         <f>(N36-P36)/P36</f>
         <v>5.5138230799848457E-4</v>
       </c>
-      <c r="S40" s="5" t="s">
+      <c r="S40" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="T40" s="6">
+      <c r="T40" s="5">
         <f>(U36-T36)/T36</f>
         <v>-7.6461969280720063E-2</v>
       </c>
-      <c r="U40" s="6"/>
-      <c r="V40" s="6">
+      <c r="U40" s="5"/>
+      <c r="V40" s="5">
         <f>(U36-V36)/V36</f>
         <v>1.3258061296113018E-3</v>
       </c>
-      <c r="W40" s="6">
+      <c r="W40" s="5">
         <f>(U36-W36)/W36</f>
         <v>1.5918465000994504E-3</v>
       </c>
@@ -16144,35 +16149,35 @@
       <c r="F41">
         <v>21.985949999999999</v>
       </c>
-      <c r="L41" s="5" t="s">
+      <c r="L41" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="M41" s="6">
+      <c r="M41" s="5">
         <f>(O36-M36)/M36</f>
         <v>-0.10813911830837769</v>
       </c>
-      <c r="N41" s="6">
+      <c r="N41" s="5">
         <f>(O36-N36)/N36</f>
         <v>-6.3706414558329879E-4</v>
       </c>
-      <c r="O41" s="6"/>
-      <c r="P41" s="6">
+      <c r="O41" s="5"/>
+      <c r="P41" s="5">
         <f>(O36-P36)/P36</f>
         <v>-8.6033103483749057E-5</v>
       </c>
-      <c r="S41" s="5" t="s">
+      <c r="S41" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="T41" s="6">
+      <c r="T41" s="5">
         <f>(V36-T36)/T36</f>
         <v>-7.7684780452230276E-2</v>
       </c>
-      <c r="U41" s="6">
+      <c r="U41" s="5">
         <f>(V36-U36)/U36</f>
         <v>-1.3240506950838436E-3</v>
       </c>
-      <c r="V41" s="6"/>
-      <c r="W41" s="6">
+      <c r="V41" s="5"/>
+      <c r="W41" s="5">
         <f>(V36-W36)/W36</f>
         <v>2.6568811955068341E-4</v>
       </c>
@@ -16193,190 +16198,190 @@
       <c r="F42">
         <v>21.985949999999999</v>
       </c>
-      <c r="L42" s="5" t="s">
+      <c r="L42" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="M42" s="6">
+      <c r="M42" s="5">
         <f>(P36-M36)/M36</f>
         <v>-0.1080623821469999</v>
       </c>
-      <c r="N42" s="6">
+      <c r="N42" s="5">
         <f>(P36-N36)/N36</f>
         <v>-5.5107845308913195E-4</v>
       </c>
-      <c r="O42" s="6">
+      <c r="O42" s="5">
         <f>(P36-O36)/O36</f>
         <v>8.6040505815489668E-5</v>
       </c>
-      <c r="P42" s="5"/>
-      <c r="S42" s="5" t="s">
+      <c r="P42" s="4"/>
+      <c r="S42" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="T42" s="6">
+      <c r="T42" s="5">
         <f>(W36-T36)/T36</f>
         <v>-7.7929763559443824E-2</v>
       </c>
-      <c r="U42" s="6">
+      <c r="U42" s="5">
         <f>(W36-U36)/U36</f>
         <v>-1.5893165521084264E-3</v>
       </c>
-      <c r="V42" s="6">
+      <c r="V42" s="5">
         <f>(W36-V36)/V36</f>
         <v>-2.6561754812380275E-4</v>
       </c>
-      <c r="W42" s="5"/>
+      <c r="W42" s="4"/>
     </row>
     <row r="43" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="L43" s="7" t="s">
+      <c r="L43" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="M43" s="7"/>
-      <c r="N43" s="7"/>
-      <c r="O43" s="7"/>
-      <c r="P43" s="7"/>
-      <c r="S43" s="7" t="s">
+      <c r="M43" s="9"/>
+      <c r="N43" s="9"/>
+      <c r="O43" s="9"/>
+      <c r="P43" s="9"/>
+      <c r="S43" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="T43" s="7"/>
-      <c r="U43" s="7"/>
-      <c r="V43" s="7"/>
-      <c r="W43" s="7"/>
+      <c r="T43" s="9"/>
+      <c r="U43" s="9"/>
+      <c r="V43" s="9"/>
+      <c r="W43" s="9"/>
     </row>
     <row r="44" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="L44" s="5" t="s">
+      <c r="L44" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="M44" s="5"/>
-      <c r="N44" s="6">
+      <c r="M44" s="4"/>
+      <c r="N44" s="5">
         <f>(M35-N35)/N35</f>
         <v>0.14544563775119065</v>
       </c>
-      <c r="O44" s="6">
+      <c r="O44" s="5">
         <f>(M35-O35)/O35</f>
         <v>0.15413383185266477</v>
       </c>
-      <c r="P44" s="6">
+      <c r="P44" s="5">
         <f>(M35-P35)/P35</f>
         <v>0.15472729642334282</v>
       </c>
-      <c r="S44" s="5" t="s">
+      <c r="S44" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="T44" s="5"/>
-      <c r="U44" s="6">
+      <c r="T44" s="4"/>
+      <c r="U44" s="5">
         <f>(T35-U35)/U35</f>
         <v>0.11420198025618267</v>
       </c>
-      <c r="V44" s="6">
+      <c r="V44" s="5">
         <f>(T35-V35)/V35</f>
         <v>0.13365320742694087</v>
       </c>
-      <c r="W44" s="6">
+      <c r="W44" s="5">
         <f>(T35-W35)/W35</f>
         <v>0.1345775442192606</v>
       </c>
     </row>
     <row r="45" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="L45" s="5" t="s">
+      <c r="L45" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="M45" s="6">
+      <c r="M45" s="5">
         <f>(N35-M35)/M35</f>
         <v>-0.12697733786540796</v>
       </c>
-      <c r="N45" s="5"/>
-      <c r="O45" s="6">
+      <c r="N45" s="4"/>
+      <c r="O45" s="5">
         <f>(N35-O35)/O35</f>
         <v>7.584990343610991E-3</v>
       </c>
-      <c r="P45" s="6">
+      <c r="P45" s="5">
         <f>(N35-P35)/P35</f>
         <v>8.1030983629869074E-3</v>
       </c>
-      <c r="S45" s="5" t="s">
+      <c r="S45" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="T45" s="6">
+      <c r="T45" s="5">
         <f>(U35-T35)/T35</f>
         <v>-0.10249665884629357</v>
       </c>
-      <c r="U45" s="5"/>
-      <c r="V45" s="6">
+      <c r="U45" s="4"/>
+      <c r="V45" s="5">
         <f>(U35-V35)/V35</f>
         <v>1.7457541375295246E-2</v>
       </c>
-      <c r="W45" s="6">
+      <c r="W45" s="5">
         <f>(U35-W35)/W35</f>
         <v>1.82871367347535E-2</v>
       </c>
     </row>
     <row r="46" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="L46" s="5" t="s">
+      <c r="L46" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="M46" s="6">
+      <c r="M46" s="5">
         <f>(O35-M35)/M35</f>
         <v>-0.1335493576210677</v>
       </c>
-      <c r="N46" s="6">
+      <c r="N46" s="5">
         <f>(O35-N35)/N35</f>
         <v>-7.5278913603350969E-3</v>
       </c>
-      <c r="O46" s="5"/>
-      <c r="P46" s="6">
+      <c r="O46" s="4"/>
+      <c r="P46" s="5">
         <f>(O35-P35)/P35</f>
         <v>5.1420775849313519E-4</v>
       </c>
-      <c r="S46" s="5" t="s">
+      <c r="S46" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="T46" s="6">
+      <c r="T46" s="5">
         <f>(V35-T35)/T35</f>
         <v>-0.11789602547880962</v>
       </c>
-      <c r="U46" s="6">
+      <c r="U46" s="5">
         <f>(V35-U35)/U35</f>
         <v>-1.7158004796640383E-2</v>
       </c>
-      <c r="V46" s="5"/>
-      <c r="W46" s="6">
+      <c r="V46" s="4"/>
+      <c r="W46" s="5">
         <f>(V35-W35)/W35</f>
         <v>8.1536115830139956E-4</v>
       </c>
     </row>
     <row r="47" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="L47" s="5" t="s">
+      <c r="L47" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="M47" s="6">
+      <c r="M47" s="5">
         <f>(P35-M35)/M35</f>
         <v>-0.13399466428358955</v>
       </c>
-      <c r="N47" s="6">
+      <c r="N47" s="5">
         <f>(P35-N35)/N35</f>
         <v>-8.0379659343822688E-3</v>
       </c>
-      <c r="O47" s="6">
+      <c r="O47" s="5">
         <f>(P35-O35)/O35</f>
         <v>-5.1394348476584161E-4</v>
       </c>
-      <c r="P47" s="5"/>
-      <c r="S47" s="5" t="s">
+      <c r="P47" s="4"/>
+      <c r="S47" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="T47" s="6">
+      <c r="T47" s="5">
         <f>(W35-T35)/T35</f>
         <v>-0.1186146728400726</v>
       </c>
-      <c r="U47" s="6">
+      <c r="U47" s="5">
         <f>(W35-U35)/U35</f>
         <v>-1.7958723109665471E-2</v>
       </c>
-      <c r="V47" s="6">
+      <c r="V47" s="5">
         <f>(W35-V35)/V35</f>
         <v>-8.1469688610468079E-4</v>
       </c>
-      <c r="W47" s="5"/>
+      <c r="W47" s="4"/>
     </row>
     <row r="48" spans="1:23" x14ac:dyDescent="0.25">
       <c r="M48" s="2"/>
@@ -16551,13 +16556,13 @@
       </c>
     </row>
     <row r="55" spans="12:23" x14ac:dyDescent="0.25">
-      <c r="L55" s="4" t="s">
+      <c r="L55" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="M55" s="4"/>
-      <c r="N55" s="4"/>
-      <c r="O55" s="4"/>
-      <c r="P55" s="4"/>
+      <c r="M55" s="8"/>
+      <c r="N55" s="8"/>
+      <c r="O55" s="8"/>
+      <c r="P55" s="8"/>
       <c r="S55" t="s">
         <v>60</v>
       </c>
@@ -16579,301 +16584,301 @@
       </c>
     </row>
     <row r="56" spans="12:23" x14ac:dyDescent="0.25">
-      <c r="L56" s="5" t="s">
+      <c r="L56" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="M56" s="6"/>
-      <c r="N56" s="6">
+      <c r="M56" s="5"/>
+      <c r="N56" s="5">
         <f>(M53-N53)/N53</f>
         <v>1.1939635950889808E-2</v>
       </c>
-      <c r="O56" s="6">
+      <c r="O56" s="5">
         <f>(M53-O53)/O53</f>
         <v>3.3911691312952801E-3</v>
       </c>
-      <c r="P56" s="6">
+      <c r="P56" s="5">
         <f>(M53-P53)/P53</f>
         <v>-1.6294443460130585E-2</v>
       </c>
-      <c r="S56" s="4" t="s">
+      <c r="S56" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="T56" s="4"/>
-      <c r="U56" s="4"/>
-      <c r="V56" s="4"/>
-      <c r="W56" s="4"/>
+      <c r="T56" s="8"/>
+      <c r="U56" s="8"/>
+      <c r="V56" s="8"/>
+      <c r="W56" s="8"/>
     </row>
     <row r="57" spans="12:23" x14ac:dyDescent="0.25">
-      <c r="L57" s="5" t="s">
+      <c r="L57" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="M57" s="6">
+      <c r="M57" s="5">
         <f>(N53-M53)/M53</f>
         <v>-1.1798763015810211E-2</v>
       </c>
-      <c r="N57" s="6"/>
-      <c r="O57" s="6">
+      <c r="N57" s="5"/>
+      <c r="O57" s="5">
         <f>(N53-O53)/O53</f>
         <v>-8.4476054854416144E-3</v>
       </c>
-      <c r="P57" s="6">
+      <c r="P57" s="5">
         <f>(N53-P53)/P53</f>
         <v>-2.7900952199080196E-2</v>
       </c>
-      <c r="S57" s="5" t="s">
+      <c r="S57" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="T57" s="6"/>
-      <c r="U57" s="6">
+      <c r="T57" s="5"/>
+      <c r="U57" s="5">
         <f>(T54-U54)/U54</f>
         <v>6.9374012236377444E-2</v>
       </c>
-      <c r="V57" s="6">
+      <c r="V57" s="5">
         <f>(T54-V54)/V54</f>
         <v>6.6347157065589302E-2</v>
       </c>
-      <c r="W57" s="6">
+      <c r="W57" s="5">
         <f>(T54-W54)/W54</f>
         <v>7.3203984343978318E-2</v>
       </c>
     </row>
     <row r="58" spans="12:23" x14ac:dyDescent="0.25">
-      <c r="L58" s="5" t="s">
+      <c r="L58" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="M58" s="6">
+      <c r="M58" s="5">
         <f>(O53-M53)/M53</f>
         <v>-3.3797079699547771E-3</v>
       </c>
-      <c r="N58" s="6">
+      <c r="N58" s="5">
         <f>(O53-N53)/N53</f>
         <v>8.5195754981534505E-3</v>
       </c>
-      <c r="O58" s="6"/>
-      <c r="P58" s="6">
+      <c r="O58" s="5"/>
+      <c r="P58" s="5">
         <f>(O53-P53)/P53</f>
         <v>-1.9619080969657181E-2</v>
       </c>
-      <c r="S58" s="5" t="s">
+      <c r="S58" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="T58" s="6">
+      <c r="T58" s="5">
         <f>(U54-T54)/T54</f>
         <v>-6.4873478729201448E-2</v>
       </c>
-      <c r="U58" s="6"/>
-      <c r="V58" s="6">
+      <c r="U58" s="5"/>
+      <c r="V58" s="5">
         <f>(U54-V54)/V54</f>
         <v>-2.8304925462496371E-3</v>
       </c>
-      <c r="W58" s="6">
+      <c r="W58" s="5">
         <f>(U54-W54)/W54</f>
         <v>3.5815084935449989E-3</v>
       </c>
     </row>
     <row r="59" spans="12:23" x14ac:dyDescent="0.25">
-      <c r="L59" s="5" t="s">
+      <c r="L59" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="M59" s="6">
+      <c r="M59" s="5">
         <f>(P53-M53)/M53</f>
         <v>1.656435033003717E-2</v>
       </c>
-      <c r="N59" s="6">
+      <c r="N59" s="5">
         <f>(P53-N53)/N53</f>
         <v>2.8701758593630625E-2</v>
       </c>
-      <c r="O59" s="6">
+      <c r="O59" s="5">
         <f>(P53-O53)/O53</f>
         <v>2.0011691974851635E-2</v>
       </c>
-      <c r="P59" s="5"/>
-      <c r="S59" s="5" t="s">
+      <c r="P59" s="4"/>
+      <c r="S59" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="T59" s="6">
+      <c r="T59" s="5">
         <f>(V54-T54)/T54</f>
         <v>-6.2219096872884891E-2</v>
       </c>
-      <c r="U59" s="6">
+      <c r="U59" s="5">
         <f>(V54-U54)/U54</f>
         <v>2.838526975696675E-3</v>
       </c>
-      <c r="V59" s="6"/>
-      <c r="W59" s="6">
+      <c r="V59" s="5"/>
+      <c r="W59" s="5">
         <f>(V54-W54)/W54</f>
         <v>6.4302016777142883E-3</v>
       </c>
     </row>
     <row r="60" spans="12:23" x14ac:dyDescent="0.25">
-      <c r="L60" s="7" t="s">
+      <c r="L60" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="M60" s="7"/>
-      <c r="N60" s="7"/>
-      <c r="O60" s="7"/>
-      <c r="P60" s="7"/>
-      <c r="S60" s="5" t="s">
+      <c r="M60" s="9"/>
+      <c r="N60" s="9"/>
+      <c r="O60" s="9"/>
+      <c r="P60" s="9"/>
+      <c r="S60" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="T60" s="6">
+      <c r="T60" s="5">
         <f>(W54-T54)/T54</f>
         <v>-6.8210690056956888E-2</v>
       </c>
-      <c r="U60" s="6">
+      <c r="U60" s="5">
         <f>(W54-U54)/U54</f>
         <v>-3.5687270672425256E-3</v>
       </c>
-      <c r="V60" s="6">
+      <c r="V60" s="5">
         <f>(W54-V54)/V54</f>
         <v>-6.3891183581287333E-3</v>
       </c>
-      <c r="W60" s="5"/>
+      <c r="W60" s="4"/>
     </row>
     <row r="61" spans="12:23" x14ac:dyDescent="0.25">
-      <c r="L61" s="5" t="s">
+      <c r="L61" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="M61" s="5"/>
-      <c r="N61" s="6">
+      <c r="M61" s="4"/>
+      <c r="N61" s="5">
         <f>(M52-N52)/N52</f>
         <v>4.4677756046552136E-2</v>
       </c>
-      <c r="O61" s="6">
+      <c r="O61" s="5">
         <f>(M52-O52)/O52</f>
         <v>0.10290136294934353</v>
       </c>
-      <c r="P61" s="6">
+      <c r="P61" s="5">
         <f>(M52-P52)/P52</f>
         <v>0.10117783207669008</v>
       </c>
-      <c r="S61" s="7" t="s">
+      <c r="S61" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="T61" s="7"/>
-      <c r="U61" s="7"/>
-      <c r="V61" s="7"/>
-      <c r="W61" s="7"/>
+      <c r="T61" s="9"/>
+      <c r="U61" s="9"/>
+      <c r="V61" s="9"/>
+      <c r="W61" s="9"/>
     </row>
     <row r="62" spans="12:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="L62" s="5" t="s">
+      <c r="L62" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="M62" s="6">
+      <c r="M62" s="5">
         <f>(N52-M52)/M52</f>
         <v>-4.2767021493430972E-2</v>
       </c>
-      <c r="N62" s="5"/>
-      <c r="O62" s="6">
+      <c r="N62" s="4"/>
+      <c r="O62" s="5">
         <f>(N52-O52)/O52</f>
         <v>5.5733556654954643E-2</v>
       </c>
-      <c r="P62" s="6">
+      <c r="P62" s="5">
         <f>(N52-P52)/P52</f>
         <v>5.408373606417656E-2</v>
       </c>
-      <c r="S62" s="5" t="s">
+      <c r="S62" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="T62" s="5"/>
-      <c r="U62" s="6">
+      <c r="T62" s="4"/>
+      <c r="U62" s="5">
         <f>(T53-U53)/U53</f>
         <v>0.10972230995351735</v>
       </c>
-      <c r="V62" s="6">
+      <c r="V62" s="5">
         <f>(T53-V53)/V53</f>
         <v>0.10328758148801032</v>
       </c>
-      <c r="W62" s="6">
+      <c r="W62" s="5">
         <f>(T53-W53)/W53</f>
         <v>0.11836270058660391</v>
       </c>
     </row>
     <row r="63" spans="12:23" x14ac:dyDescent="0.25">
-      <c r="L63" s="5" t="s">
+      <c r="L63" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="M63" s="6">
+      <c r="M63" s="5">
         <f>(O52-M52)/M52</f>
         <v>-9.330060366791823E-2</v>
       </c>
-      <c r="N63" s="6">
+      <c r="N63" s="5">
         <f>(O52-N52)/N52</f>
         <v>-5.2791309231037385E-2</v>
       </c>
-      <c r="O63" s="5"/>
-      <c r="P63" s="6">
+      <c r="O63" s="4"/>
+      <c r="P63" s="5">
         <f>(O52-P52)/P52</f>
         <v>-1.5627244017945823E-3</v>
       </c>
-      <c r="S63" s="5" t="s">
+      <c r="S63" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="T63" s="6">
+      <c r="T63" s="5">
         <f>(U53-T53)/T53</f>
         <v>-9.8873663230320444E-2</v>
       </c>
-      <c r="U63" s="5"/>
-      <c r="V63" s="6">
+      <c r="U63" s="4"/>
+      <c r="V63" s="5">
         <f>(U53-V53)/V53</f>
         <v>-5.7985032902299416E-3</v>
       </c>
-      <c r="W63" s="6">
+      <c r="W63" s="5">
         <f>(U53-W53)/W53</f>
         <v>7.7860835594523413E-3</v>
       </c>
     </row>
     <row r="64" spans="12:23" x14ac:dyDescent="0.25">
-      <c r="L64" s="5" t="s">
+      <c r="L64" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="M64" s="6">
+      <c r="M64" s="5">
         <f>(P52-M52)/M52</f>
         <v>-9.1881464673040827E-2</v>
       </c>
-      <c r="N64" s="6">
+      <c r="N64" s="5">
         <f>(P52-N52)/N52</f>
         <v>-5.1308766290350714E-2</v>
       </c>
-      <c r="O64" s="6">
+      <c r="O64" s="5">
         <f>(P52-O52)/O52</f>
         <v>1.5651703316648397E-3</v>
       </c>
-      <c r="P64" s="5"/>
-      <c r="S64" s="5" t="s">
+      <c r="P64" s="4"/>
+      <c r="S64" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="T64" s="6">
+      <c r="T64" s="5">
         <f>(V53-T53)/T53</f>
         <v>-9.3618004245734146E-2</v>
       </c>
-      <c r="U64" s="6">
+      <c r="U64" s="5">
         <f>(V53-U53)/U53</f>
         <v>5.8323220287030573E-3</v>
       </c>
-      <c r="V64" s="5"/>
-      <c r="W64" s="6">
+      <c r="V64" s="4"/>
+      <c r="W64" s="5">
         <f>(V53-W53)/W53</f>
         <v>1.3663816534816514E-2</v>
       </c>
     </row>
     <row r="65" spans="19:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="S65" s="5" t="s">
+      <c r="S65" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="T65" s="6">
+      <c r="T65" s="5">
         <f>(W53-T53)/T53</f>
         <v>-0.1058357011768367</v>
       </c>
-      <c r="U65" s="6">
+      <c r="U65" s="5">
         <f>(W53-U53)/U53</f>
         <v>-7.725928831992069E-3</v>
       </c>
-      <c r="V65" s="6">
+      <c r="V65" s="5">
         <f>(W53-V53)/V53</f>
         <v>-1.3479633298469624E-2</v>
       </c>
-      <c r="W65" s="5"/>
+      <c r="W65" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -18135,13 +18140,13 @@
       <c r="J36">
         <v>28.283641966836871</v>
       </c>
-      <c r="L36" s="4" t="s">
+      <c r="L36" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="M36" s="4"/>
-      <c r="N36" s="4"/>
-      <c r="O36" s="4"/>
-      <c r="P36" s="4"/>
+      <c r="M36" s="8"/>
+      <c r="N36" s="8"/>
+      <c r="O36" s="8"/>
+      <c r="P36" s="8"/>
     </row>
     <row r="37" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
@@ -18174,19 +18179,19 @@
       <c r="J37">
         <v>44.455277770153181</v>
       </c>
-      <c r="L37" s="5" t="s">
+      <c r="L37" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="M37" s="6"/>
-      <c r="N37" s="6">
+      <c r="M37" s="5"/>
+      <c r="N37" s="5">
         <f>(M34-N34)/N34</f>
         <v>0.12053679712792387</v>
       </c>
-      <c r="O37" s="6">
+      <c r="O37" s="5">
         <f>(M34-O34)/O34</f>
         <v>0.12125110600575575</v>
       </c>
-      <c r="P37" s="6">
+      <c r="P37" s="5">
         <f>(M34-P34)/P34</f>
         <v>0.1211546412933215</v>
       </c>
@@ -18204,19 +18209,19 @@
       <c r="F38">
         <v>18.391079999999999</v>
       </c>
-      <c r="L38" s="5" t="s">
+      <c r="L38" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="M38" s="6">
+      <c r="M38" s="5">
         <f>(N34-M34)/M34</f>
         <v>-0.10757058352467744</v>
       </c>
-      <c r="N38" s="6"/>
-      <c r="O38" s="6">
+      <c r="N38" s="5"/>
+      <c r="O38" s="5">
         <f>(N34-O34)/O34</f>
         <v>6.3747025502665215E-4</v>
       </c>
-      <c r="P38" s="6">
+      <c r="P38" s="5">
         <f>(N34-P34)/P34</f>
         <v>5.5138230799848457E-4</v>
       </c>
@@ -18234,19 +18239,19 @@
       <c r="F39">
         <v>18.391079999999999</v>
       </c>
-      <c r="L39" s="5" t="s">
+      <c r="L39" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="M39" s="6">
+      <c r="M39" s="5">
         <f>(O34-M34)/M34</f>
         <v>-0.10813911830837769</v>
       </c>
-      <c r="N39" s="6">
+      <c r="N39" s="5">
         <f>(O34-N34)/N34</f>
         <v>-6.3706414558329879E-4</v>
       </c>
-      <c r="O39" s="6"/>
-      <c r="P39" s="6">
+      <c r="O39" s="5"/>
+      <c r="P39" s="5">
         <f>(O34-P34)/P34</f>
         <v>-8.6033103483749057E-5</v>
       </c>
@@ -18264,22 +18269,22 @@
       <c r="F40">
         <v>18.391079999999999</v>
       </c>
-      <c r="L40" s="5" t="s">
+      <c r="L40" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="M40" s="6">
+      <c r="M40" s="5">
         <f>(P34-M34)/M34</f>
         <v>-0.1080623821469999</v>
       </c>
-      <c r="N40" s="6">
+      <c r="N40" s="5">
         <f>(P34-N34)/N34</f>
         <v>-5.5107845308913195E-4</v>
       </c>
-      <c r="O40" s="6">
+      <c r="O40" s="5">
         <f>(P34-O34)/O34</f>
         <v>8.6040505815489668E-5</v>
       </c>
-      <c r="P40" s="5"/>
+      <c r="P40" s="4"/>
     </row>
     <row r="41" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C41">
@@ -18294,13 +18299,13 @@
       <c r="F41">
         <v>18.391079999999999</v>
       </c>
-      <c r="L41" s="7" t="s">
+      <c r="L41" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="M41" s="7"/>
-      <c r="N41" s="7"/>
-      <c r="O41" s="7"/>
-      <c r="P41" s="7"/>
+      <c r="M41" s="9"/>
+      <c r="N41" s="9"/>
+      <c r="O41" s="9"/>
+      <c r="P41" s="9"/>
     </row>
     <row r="42" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C42">
@@ -18315,76 +18320,76 @@
       <c r="F42">
         <v>18.391079999999999</v>
       </c>
-      <c r="L42" s="5" t="s">
+      <c r="L42" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="M42" s="5"/>
-      <c r="N42" s="6">
+      <c r="M42" s="4"/>
+      <c r="N42" s="5">
         <f>(M33-N33)/N33</f>
         <v>0.14544563775119065</v>
       </c>
-      <c r="O42" s="6">
+      <c r="O42" s="5">
         <f>(M33-O33)/O33</f>
         <v>0.15413383185266477</v>
       </c>
-      <c r="P42" s="6">
+      <c r="P42" s="5">
         <f>(M33-P33)/P33</f>
         <v>0.15472729642334282</v>
       </c>
     </row>
     <row r="43" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="L43" s="5" t="s">
+      <c r="L43" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="M43" s="6">
+      <c r="M43" s="5">
         <f>(N33-M33)/M33</f>
         <v>-0.12697733786540796</v>
       </c>
-      <c r="N43" s="5"/>
-      <c r="O43" s="6">
+      <c r="N43" s="4"/>
+      <c r="O43" s="5">
         <f>(N33-O33)/O33</f>
         <v>7.584990343610991E-3</v>
       </c>
-      <c r="P43" s="6">
+      <c r="P43" s="5">
         <f>(N33-P33)/P33</f>
         <v>8.1030983629869074E-3</v>
       </c>
     </row>
     <row r="44" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="L44" s="5" t="s">
+      <c r="L44" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="M44" s="6">
+      <c r="M44" s="5">
         <f>(O33-M33)/M33</f>
         <v>-0.1335493576210677</v>
       </c>
-      <c r="N44" s="6">
+      <c r="N44" s="5">
         <f>(O33-N33)/N33</f>
         <v>-7.5278913603350969E-3</v>
       </c>
-      <c r="O44" s="5"/>
-      <c r="P44" s="6">
+      <c r="O44" s="4"/>
+      <c r="P44" s="5">
         <f>(O33-P33)/P33</f>
         <v>5.1420775849313519E-4</v>
       </c>
     </row>
     <row r="45" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="L45" s="5" t="s">
+      <c r="L45" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="M45" s="6">
+      <c r="M45" s="5">
         <f>(P33-M33)/M33</f>
         <v>-0.13399466428358955</v>
       </c>
-      <c r="N45" s="6">
+      <c r="N45" s="5">
         <f>(P33-N33)/N33</f>
         <v>-8.0379659343822688E-3</v>
       </c>
-      <c r="O45" s="6">
+      <c r="O45" s="5">
         <f>(P33-O33)/O33</f>
         <v>-5.1394348476584161E-4</v>
       </c>
-      <c r="P45" s="5"/>
+      <c r="P45" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -19470,13 +19475,13 @@
       <c r="I34">
         <v>-14.94128081710544</v>
       </c>
-      <c r="K34" s="4" t="s">
+      <c r="K34" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="L34" s="4"/>
-      <c r="M34" s="4"/>
-      <c r="N34" s="4"/>
-      <c r="O34" s="4"/>
+      <c r="L34" s="8"/>
+      <c r="M34" s="8"/>
+      <c r="N34" s="8"/>
+      <c r="O34" s="8"/>
     </row>
     <row r="35" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A35">
@@ -19506,19 +19511,19 @@
       <c r="I35">
         <v>-12.70008869453962</v>
       </c>
-      <c r="K35" s="5" t="s">
+      <c r="K35" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="L35" s="6"/>
-      <c r="M35" s="6">
+      <c r="L35" s="5"/>
+      <c r="M35" s="5">
         <f>(L32-M32)/M32</f>
         <v>8.2792442473829816E-2</v>
       </c>
-      <c r="N35" s="6">
+      <c r="N35" s="5">
         <f>(L32-N32)/N32</f>
         <v>8.422801533115841E-2</v>
       </c>
-      <c r="O35" s="6">
+      <c r="O35" s="5">
         <f>(L32-O32)/O32</f>
         <v>8.4516081833715909E-2</v>
       </c>
@@ -19551,19 +19556,19 @@
       <c r="I36">
         <v>30.204924609641321</v>
       </c>
-      <c r="K36" s="5" t="s">
+      <c r="K36" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="L36" s="6">
+      <c r="L36" s="5">
         <f>(M32-L32)/L32</f>
         <v>-7.6461969280720063E-2</v>
       </c>
-      <c r="M36" s="6"/>
-      <c r="N36" s="6">
+      <c r="M36" s="5"/>
+      <c r="N36" s="5">
         <f>(M32-N32)/N32</f>
         <v>1.3258061296113018E-3</v>
       </c>
-      <c r="O36" s="6">
+      <c r="O36" s="5">
         <f>(M32-O32)/O32</f>
         <v>1.5918465000994504E-3</v>
       </c>
@@ -19596,19 +19601,19 @@
       <c r="I37">
         <v>44.674185918195121</v>
       </c>
-      <c r="K37" s="5" t="s">
+      <c r="K37" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="L37" s="6">
+      <c r="L37" s="5">
         <f>(N32-L32)/L32</f>
         <v>-7.7684780452230276E-2</v>
       </c>
-      <c r="M37" s="6">
+      <c r="M37" s="5">
         <f>(N32-M32)/M32</f>
         <v>-1.3240506950838436E-3</v>
       </c>
-      <c r="N37" s="6"/>
-      <c r="O37" s="6">
+      <c r="N37" s="5"/>
+      <c r="O37" s="5">
         <f>(N32-O32)/O32</f>
         <v>2.6568811955068341E-4</v>
       </c>
@@ -19626,22 +19631,22 @@
       <c r="E38">
         <v>18.380500000000001</v>
       </c>
-      <c r="K38" s="5" t="s">
+      <c r="K38" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="L38" s="6">
+      <c r="L38" s="5">
         <f>(O32-L32)/L32</f>
         <v>-7.7929763559443824E-2</v>
       </c>
-      <c r="M38" s="6">
+      <c r="M38" s="5">
         <f>(O32-M32)/M32</f>
         <v>-1.5893165521084264E-3</v>
       </c>
-      <c r="N38" s="6">
+      <c r="N38" s="5">
         <f>(O32-N32)/N32</f>
         <v>-2.6561754812380275E-4</v>
       </c>
-      <c r="O38" s="5"/>
+      <c r="O38" s="4"/>
     </row>
     <row r="39" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B39">
@@ -19656,13 +19661,13 @@
       <c r="E39">
         <v>18.380500000000001</v>
       </c>
-      <c r="K39" s="7" t="s">
+      <c r="K39" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="L39" s="7"/>
-      <c r="M39" s="7"/>
-      <c r="N39" s="7"/>
-      <c r="O39" s="7"/>
+      <c r="L39" s="9"/>
+      <c r="M39" s="9"/>
+      <c r="N39" s="9"/>
+      <c r="O39" s="9"/>
     </row>
     <row r="40" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B40">
@@ -19677,19 +19682,19 @@
       <c r="E40">
         <v>18.380500000000001</v>
       </c>
-      <c r="K40" s="5" t="s">
+      <c r="K40" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="L40" s="5"/>
-      <c r="M40" s="6">
+      <c r="L40" s="4"/>
+      <c r="M40" s="5">
         <f>(L31-M31)/M31</f>
         <v>0.11420198025618267</v>
       </c>
-      <c r="N40" s="6">
+      <c r="N40" s="5">
         <f>(L31-N31)/N31</f>
         <v>0.13365320742694087</v>
       </c>
-      <c r="O40" s="6">
+      <c r="O40" s="5">
         <f>(L31-O31)/O31</f>
         <v>0.1345775442192606</v>
       </c>
@@ -19707,19 +19712,19 @@
       <c r="E41">
         <v>18.380500000000001</v>
       </c>
-      <c r="K41" s="5" t="s">
+      <c r="K41" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="L41" s="6">
+      <c r="L41" s="5">
         <f>(M31-L31)/L31</f>
         <v>-0.10249665884629357</v>
       </c>
-      <c r="M41" s="5"/>
-      <c r="N41" s="6">
+      <c r="M41" s="4"/>
+      <c r="N41" s="5">
         <f>(M31-N31)/N31</f>
         <v>1.7457541375295246E-2</v>
       </c>
-      <c r="O41" s="6">
+      <c r="O41" s="5">
         <f>(M31-O31)/O31</f>
         <v>1.82871367347535E-2</v>
       </c>
@@ -19737,40 +19742,40 @@
       <c r="E42">
         <v>18.380500000000001</v>
       </c>
-      <c r="K42" s="5" t="s">
+      <c r="K42" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="L42" s="6">
+      <c r="L42" s="5">
         <f>(N31-L31)/L31</f>
         <v>-0.11789602547880962</v>
       </c>
-      <c r="M42" s="6">
+      <c r="M42" s="5">
         <f>(N31-M31)/M31</f>
         <v>-1.7158004796640383E-2</v>
       </c>
-      <c r="N42" s="5"/>
-      <c r="O42" s="6">
+      <c r="N42" s="4"/>
+      <c r="O42" s="5">
         <f>(N31-O31)/O31</f>
         <v>8.1536115830139956E-4</v>
       </c>
     </row>
     <row r="43" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="K43" s="5" t="s">
+      <c r="K43" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="L43" s="6">
+      <c r="L43" s="5">
         <f>(O31-L31)/L31</f>
         <v>-0.1186146728400726</v>
       </c>
-      <c r="M43" s="6">
+      <c r="M43" s="5">
         <f>(O31-M31)/M31</f>
         <v>-1.7958723109665471E-2</v>
       </c>
-      <c r="N43" s="6">
+      <c r="N43" s="5">
         <f>(O31-N31)/N31</f>
         <v>-8.1469688610468079E-4</v>
       </c>
-      <c r="O43" s="5"/>
+      <c r="O43" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -20863,13 +20868,13 @@
       <c r="J31">
         <v>-2.1059569045901299</v>
       </c>
-      <c r="M31" s="4" t="s">
+      <c r="M31" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="N31" s="4"/>
-      <c r="O31" s="4"/>
-      <c r="P31" s="4"/>
-      <c r="Q31" s="4"/>
+      <c r="N31" s="8"/>
+      <c r="O31" s="8"/>
+      <c r="P31" s="8"/>
+      <c r="Q31" s="8"/>
     </row>
     <row r="32" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
@@ -20902,20 +20907,20 @@
       <c r="J32">
         <v>-6.0529784522950649</v>
       </c>
-      <c r="L32" s="8"/>
-      <c r="M32" s="5" t="s">
+      <c r="L32" s="6"/>
+      <c r="M32" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="N32" s="6"/>
-      <c r="O32" s="6">
+      <c r="N32" s="5"/>
+      <c r="O32" s="5">
         <f>(N29-O29)/O29</f>
         <v>1.1939635950889808E-2</v>
       </c>
-      <c r="P32" s="6">
+      <c r="P32" s="5">
         <f>(N29-P29)/P29</f>
         <v>3.3911691312952801E-3</v>
       </c>
-      <c r="Q32" s="6">
+      <c r="Q32" s="5">
         <f>(N29-Q29)/Q29</f>
         <v>-1.6294443460130585E-2</v>
       </c>
@@ -20951,20 +20956,20 @@
       <c r="J33">
         <v>23.973510773852471</v>
       </c>
-      <c r="L33" s="8"/>
-      <c r="M33" s="5" t="s">
+      <c r="L33" s="6"/>
+      <c r="M33" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="N33" s="6">
+      <c r="N33" s="5">
         <f>(O29-N29)/N29</f>
         <v>-1.1798763015810211E-2</v>
       </c>
-      <c r="O33" s="6"/>
-      <c r="P33" s="6">
+      <c r="O33" s="5"/>
+      <c r="P33" s="5">
         <f>(O29-P29)/P29</f>
         <v>-8.4476054854416144E-3</v>
       </c>
-      <c r="Q33" s="6">
+      <c r="Q33" s="5">
         <f>(O29-Q29)/Q29</f>
         <v>-2.7900952199080196E-2</v>
       </c>
@@ -21000,20 +21005,20 @@
       <c r="J34">
         <v>-16.01324461307377</v>
       </c>
-      <c r="L34" s="8"/>
-      <c r="M34" s="5" t="s">
+      <c r="L34" s="6"/>
+      <c r="M34" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="N34" s="6">
+      <c r="N34" s="5">
         <f>(P29-N29)/N29</f>
         <v>-3.3797079699547771E-3</v>
       </c>
-      <c r="O34" s="6">
+      <c r="O34" s="5">
         <f>(P29-O29)/O29</f>
         <v>8.5195754981534505E-3</v>
       </c>
-      <c r="P34" s="6"/>
-      <c r="Q34" s="6">
+      <c r="P34" s="5"/>
+      <c r="Q34" s="5">
         <f>(P29-Q29)/Q29</f>
         <v>-1.9619080969657181E-2</v>
       </c>
@@ -21049,22 +21054,22 @@
       <c r="J35">
         <v>-8.0066223065368831</v>
       </c>
-      <c r="M35" s="5" t="s">
+      <c r="M35" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="N35" s="6">
+      <c r="N35" s="5">
         <f>(Q29-N29)/N29</f>
         <v>1.656435033003717E-2</v>
       </c>
-      <c r="O35" s="6">
+      <c r="O35" s="5">
         <f>(Q29-O29)/O29</f>
         <v>2.8701758593630625E-2</v>
       </c>
-      <c r="P35" s="6">
+      <c r="P35" s="5">
         <f>(Q29-P29)/P29</f>
         <v>2.0011691974851635E-2</v>
       </c>
-      <c r="Q35" s="5"/>
+      <c r="Q35" s="4"/>
     </row>
     <row r="36" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
@@ -21097,13 +21102,13 @@
       <c r="J36">
         <v>36.996688846731558</v>
       </c>
-      <c r="M36" s="7" t="s">
+      <c r="M36" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="N36" s="7"/>
-      <c r="O36" s="7"/>
-      <c r="P36" s="7"/>
-      <c r="Q36" s="7"/>
+      <c r="N36" s="9"/>
+      <c r="O36" s="9"/>
+      <c r="P36" s="9"/>
+      <c r="Q36" s="9"/>
     </row>
     <row r="37" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
@@ -21136,76 +21141,76 @@
       <c r="J37">
         <v>37.498344423365779</v>
       </c>
-      <c r="M37" s="5" t="s">
+      <c r="M37" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="N37" s="5"/>
-      <c r="O37" s="6">
+      <c r="N37" s="4"/>
+      <c r="O37" s="5">
         <f>(N28-O28)/O28</f>
         <v>4.4677756046552136E-2</v>
       </c>
-      <c r="P37" s="6">
+      <c r="P37" s="5">
         <f>(N28-P28)/P28</f>
         <v>0.10290136294934353</v>
       </c>
-      <c r="Q37" s="6">
+      <c r="Q37" s="5">
         <f>(N28-Q28)/Q28</f>
         <v>0.10117783207669008</v>
       </c>
     </row>
     <row r="38" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="M38" s="5" t="s">
+      <c r="M38" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="N38" s="6">
+      <c r="N38" s="5">
         <f>(O28-N28)/N28</f>
         <v>-4.2767021493430972E-2</v>
       </c>
-      <c r="O38" s="5"/>
-      <c r="P38" s="6">
+      <c r="O38" s="4"/>
+      <c r="P38" s="5">
         <f>(O28-P28)/P28</f>
         <v>5.5733556654954643E-2</v>
       </c>
-      <c r="Q38" s="6">
+      <c r="Q38" s="5">
         <f>(O28-Q28)/Q28</f>
         <v>5.408373606417656E-2</v>
       </c>
     </row>
     <row r="39" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="M39" s="5" t="s">
+      <c r="M39" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="N39" s="6">
+      <c r="N39" s="5">
         <f>(P28-N28)/N28</f>
         <v>-9.330060366791823E-2</v>
       </c>
-      <c r="O39" s="6">
+      <c r="O39" s="5">
         <f>(P28-O28)/O28</f>
         <v>-5.2791309231037385E-2</v>
       </c>
-      <c r="P39" s="5"/>
-      <c r="Q39" s="6">
+      <c r="P39" s="4"/>
+      <c r="Q39" s="5">
         <f>(P28-Q28)/Q28</f>
         <v>-1.5627244017945823E-3</v>
       </c>
     </row>
     <row r="40" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="M40" s="5" t="s">
+      <c r="M40" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="N40" s="6">
+      <c r="N40" s="5">
         <f>(Q28-N28)/N28</f>
         <v>-9.1881464673040827E-2</v>
       </c>
-      <c r="O40" s="6">
+      <c r="O40" s="5">
         <f>(Q28-O28)/O28</f>
         <v>-5.1308766290350714E-2</v>
       </c>
-      <c r="P40" s="6">
+      <c r="P40" s="5">
         <f>(Q28-P28)/P28</f>
         <v>1.5651703316648397E-3</v>
       </c>
-      <c r="Q40" s="5"/>
+      <c r="Q40" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -22440,13 +22445,13 @@
       <c r="J35">
         <v>-9.2707664974478199</v>
       </c>
-      <c r="L35" s="4" t="s">
+      <c r="L35" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="M35" s="4"/>
-      <c r="N35" s="4"/>
-      <c r="O35" s="4"/>
-      <c r="P35" s="4"/>
+      <c r="M35" s="8"/>
+      <c r="N35" s="8"/>
+      <c r="O35" s="8"/>
+      <c r="P35" s="8"/>
     </row>
     <row r="36" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
@@ -22479,19 +22484,19 @@
       <c r="J36">
         <v>34.740653555014653</v>
       </c>
-      <c r="L36" s="5" t="s">
+      <c r="L36" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="M36" s="6"/>
-      <c r="N36" s="6">
+      <c r="M36" s="5"/>
+      <c r="N36" s="5">
         <f>(M33-N33)/N33</f>
         <v>6.9374012236377444E-2</v>
       </c>
-      <c r="O36" s="6">
+      <c r="O36" s="5">
         <f>(M33-O33)/O33</f>
         <v>6.6347157065589302E-2</v>
       </c>
-      <c r="P36" s="6">
+      <c r="P36" s="5">
         <f>(M33-P33)/P33</f>
         <v>7.3203984343978318E-2</v>
       </c>
@@ -22527,19 +22532,19 @@
       <c r="J37">
         <v>42.455858411050713</v>
       </c>
-      <c r="L37" s="5" t="s">
+      <c r="L37" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="M37" s="6">
+      <c r="M37" s="5">
         <f>(N33-M33)/M33</f>
         <v>-6.4873478729201448E-2</v>
       </c>
-      <c r="N37" s="6"/>
-      <c r="O37" s="6">
+      <c r="N37" s="5"/>
+      <c r="O37" s="5">
         <f>(N33-O33)/O33</f>
         <v>-2.8304925462496371E-3</v>
       </c>
-      <c r="P37" s="6">
+      <c r="P37" s="5">
         <f>(N33-P33)/P33</f>
         <v>3.5815084935449989E-3</v>
       </c>
@@ -22557,19 +22562,19 @@
       <c r="F38">
         <v>21.985949999999999</v>
       </c>
-      <c r="L38" s="5" t="s">
+      <c r="L38" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="M38" s="6">
+      <c r="M38" s="5">
         <f>(O33-M33)/M33</f>
         <v>-6.2219096872884891E-2</v>
       </c>
-      <c r="N38" s="6">
+      <c r="N38" s="5">
         <f>(O33-N33)/N33</f>
         <v>2.838526975696675E-3</v>
       </c>
-      <c r="O38" s="6"/>
-      <c r="P38" s="6">
+      <c r="O38" s="5"/>
+      <c r="P38" s="5">
         <f>(O33-P33)/P33</f>
         <v>6.4302016777142883E-3</v>
       </c>
@@ -22587,22 +22592,22 @@
       <c r="F39">
         <v>21.985949999999999</v>
       </c>
-      <c r="L39" s="5" t="s">
+      <c r="L39" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="M39" s="6">
+      <c r="M39" s="5">
         <f>(P33-M33)/M33</f>
         <v>-6.8210690056956888E-2</v>
       </c>
-      <c r="N39" s="6">
+      <c r="N39" s="5">
         <f>(P33-N33)/N33</f>
         <v>-3.5687270672425256E-3</v>
       </c>
-      <c r="O39" s="6">
+      <c r="O39" s="5">
         <f>(P33-O33)/O33</f>
         <v>-6.3891183581287333E-3</v>
       </c>
-      <c r="P39" s="5"/>
+      <c r="P39" s="4"/>
     </row>
     <row r="40" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C40">
@@ -22617,13 +22622,13 @@
       <c r="F40">
         <v>21.985949999999999</v>
       </c>
-      <c r="L40" s="7" t="s">
+      <c r="L40" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="M40" s="7"/>
-      <c r="N40" s="7"/>
-      <c r="O40" s="7"/>
-      <c r="P40" s="7"/>
+      <c r="M40" s="9"/>
+      <c r="N40" s="9"/>
+      <c r="O40" s="9"/>
+      <c r="P40" s="9"/>
     </row>
     <row r="41" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C41">
@@ -22638,19 +22643,19 @@
       <c r="F41">
         <v>21.985949999999999</v>
       </c>
-      <c r="L41" s="5" t="s">
+      <c r="L41" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="M41" s="5"/>
-      <c r="N41" s="6">
+      <c r="M41" s="4"/>
+      <c r="N41" s="5">
         <f>(M32-N32)/N32</f>
         <v>0.10972230995351735</v>
       </c>
-      <c r="O41" s="6">
+      <c r="O41" s="5">
         <f>(M32-O32)/O32</f>
         <v>0.10328758148801032</v>
       </c>
-      <c r="P41" s="6">
+      <c r="P41" s="5">
         <f>(M32-P32)/P32</f>
         <v>0.11836270058660391</v>
       </c>
@@ -22668,58 +22673,58 @@
       <c r="F42">
         <v>21.985949999999999</v>
       </c>
-      <c r="L42" s="5" t="s">
+      <c r="L42" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="M42" s="6">
+      <c r="M42" s="5">
         <f>(N32-M32)/M32</f>
         <v>-9.8873663230320444E-2</v>
       </c>
-      <c r="N42" s="5"/>
-      <c r="O42" s="6">
+      <c r="N42" s="4"/>
+      <c r="O42" s="5">
         <f>(N32-O32)/O32</f>
         <v>-5.7985032902299416E-3</v>
       </c>
-      <c r="P42" s="6">
+      <c r="P42" s="5">
         <f>(N32-P32)/P32</f>
         <v>7.7860835594523413E-3</v>
       </c>
     </row>
     <row r="43" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="L43" s="5" t="s">
+      <c r="L43" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="M43" s="6">
+      <c r="M43" s="5">
         <f>(O32-M32)/M32</f>
         <v>-9.3618004245734146E-2</v>
       </c>
-      <c r="N43" s="6">
+      <c r="N43" s="5">
         <f>(O32-N32)/N32</f>
         <v>5.8323220287030573E-3</v>
       </c>
-      <c r="O43" s="5"/>
-      <c r="P43" s="6">
+      <c r="O43" s="4"/>
+      <c r="P43" s="5">
         <f>(O32-P32)/P32</f>
         <v>1.3663816534816514E-2</v>
       </c>
     </row>
     <row r="44" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="L44" s="5" t="s">
+      <c r="L44" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="M44" s="6">
+      <c r="M44" s="5">
         <f>(P32-M32)/M32</f>
         <v>-0.1058357011768367</v>
       </c>
-      <c r="N44" s="6">
+      <c r="N44" s="5">
         <f>(P32-N32)/N32</f>
         <v>-7.725928831992069E-3</v>
       </c>
-      <c r="O44" s="6">
+      <c r="O44" s="5">
         <f>(P32-O32)/O32</f>
         <v>-1.3479633298469624E-2</v>
       </c>
-      <c r="P44" s="5"/>
+      <c r="P44" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -22733,22 +22738,19 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:N38"/>
+  <dimension ref="B1:AG39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="S37" sqref="S37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="17.42578125" customWidth="1"/>
-    <col min="4" max="4" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="14" width="4.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:33" x14ac:dyDescent="0.25">
       <c r="C1" s="10">
         <v>0.1</v>
       </c>
@@ -22765,14 +22767,14 @@
       <c r="J1" s="10"/>
       <c r="K1" s="10"/>
       <c r="L1" s="10" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="M1" s="10"/>
       <c r="N1" s="10"/>
     </row>
-    <row r="2" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:33" x14ac:dyDescent="0.25">
       <c r="C2" t="s">
-        <v>52</v>
+        <v>63</v>
       </c>
       <c r="D2" t="s">
         <v>53</v>
@@ -22781,7 +22783,7 @@
         <v>54</v>
       </c>
       <c r="F2" t="s">
-        <v>52</v>
+        <v>63</v>
       </c>
       <c r="G2" t="s">
         <v>53</v>
@@ -22790,7 +22792,7 @@
         <v>54</v>
       </c>
       <c r="I2" t="s">
-        <v>52</v>
+        <v>63</v>
       </c>
       <c r="J2" t="s">
         <v>53</v>
@@ -22799,7 +22801,7 @@
         <v>54</v>
       </c>
       <c r="L2" t="s">
-        <v>52</v>
+        <v>63</v>
       </c>
       <c r="M2" t="s">
         <v>53</v>
@@ -22807,91 +22809,90 @@
       <c r="N2" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="3" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B3" s="9">
+      <c r="AB2" t="s">
+        <v>65</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>64</v>
+      </c>
+      <c r="AE2">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="3" spans="2:33" x14ac:dyDescent="0.25">
+      <c r="B3" s="7">
         <v>44912</v>
       </c>
-      <c r="C3" t="s">
-        <v>62</v>
-      </c>
-      <c r="D3" t="s">
-        <v>62</v>
-      </c>
-      <c r="E3" t="s">
-        <v>62</v>
-      </c>
-      <c r="F3" t="s">
-        <v>62</v>
-      </c>
-      <c r="G3" t="s">
-        <v>62</v>
-      </c>
-      <c r="H3" t="s">
-        <v>62</v>
-      </c>
-      <c r="I3" t="s">
-        <v>62</v>
-      </c>
-      <c r="J3" t="s">
-        <v>62</v>
-      </c>
-      <c r="K3" t="s">
-        <v>62</v>
-      </c>
-      <c r="L3" t="s">
-        <v>62</v>
-      </c>
-      <c r="M3" t="s">
-        <v>62</v>
-      </c>
-      <c r="N3" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="4" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B4" s="9">
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
+      <c r="M3" s="2"/>
+      <c r="N3" s="2"/>
+      <c r="V3">
+        <v>0</v>
+      </c>
+      <c r="W3">
+        <v>2</v>
+      </c>
+      <c r="X3">
+        <v>2</v>
+      </c>
+      <c r="AA3">
+        <v>0</v>
+      </c>
+      <c r="AB3">
+        <v>1</v>
+      </c>
+      <c r="AC3" s="2">
+        <f>0+(($AE$2)*(AB3-0))</f>
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="4" spans="2:33" x14ac:dyDescent="0.25">
+      <c r="B4" s="7">
         <v>44579</v>
       </c>
-      <c r="C4" t="s">
-        <v>62</v>
-      </c>
-      <c r="D4" t="s">
-        <v>62</v>
-      </c>
-      <c r="E4" t="s">
-        <v>62</v>
-      </c>
-      <c r="F4" t="s">
-        <v>62</v>
-      </c>
-      <c r="G4" t="s">
-        <v>62</v>
-      </c>
-      <c r="H4" t="s">
-        <v>62</v>
-      </c>
-      <c r="I4" t="s">
-        <v>62</v>
-      </c>
-      <c r="J4" t="s">
-        <v>62</v>
-      </c>
-      <c r="K4" t="s">
-        <v>62</v>
-      </c>
-      <c r="L4" t="s">
-        <v>62</v>
-      </c>
-      <c r="M4" t="s">
-        <v>62</v>
-      </c>
-      <c r="N4" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="5" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B5" s="9">
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
+      <c r="K4" s="2"/>
+      <c r="L4" s="2"/>
+      <c r="M4" s="2"/>
+      <c r="N4" s="2"/>
+      <c r="V4">
+        <v>10</v>
+      </c>
+      <c r="W4">
+        <v>3</v>
+      </c>
+      <c r="X4">
+        <v>3</v>
+      </c>
+      <c r="AA4">
+        <v>10</v>
+      </c>
+      <c r="AB4">
+        <v>2</v>
+      </c>
+      <c r="AC4" s="2">
+        <f>AC3+(($AE$2)*(AB4-AC3))</f>
+        <v>0.29000000000000004</v>
+      </c>
+    </row>
+    <row r="5" spans="2:33" x14ac:dyDescent="0.25">
+      <c r="B5" s="7">
         <v>44610</v>
       </c>
       <c r="C5" s="2">
@@ -22930,9 +22931,29 @@
       <c r="N5" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B6" s="9">
+      <c r="V5">
+        <v>16</v>
+      </c>
+      <c r="W5">
+        <v>1</v>
+      </c>
+      <c r="X5" s="2">
+        <f>X4+(0.9*(W4-X4))</f>
+        <v>3</v>
+      </c>
+      <c r="AA5">
+        <v>16</v>
+      </c>
+      <c r="AB5">
+        <v>1</v>
+      </c>
+      <c r="AC5" s="2">
+        <f>AC4+(($AE$2)*(AB5-AC4))</f>
+        <v>0.36100000000000004</v>
+      </c>
+    </row>
+    <row r="6" spans="2:33" x14ac:dyDescent="0.25">
+      <c r="B6" s="7">
         <v>44638</v>
       </c>
       <c r="C6" s="2">
@@ -22971,9 +22992,36 @@
       <c r="N6" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B7" s="9">
+      <c r="V6">
+        <v>13</v>
+      </c>
+      <c r="W6">
+        <v>1</v>
+      </c>
+      <c r="X6" s="2">
+        <f>($AE$2*W6)+((1-$AE$2)*X5)</f>
+        <v>2.8000000000000003</v>
+      </c>
+      <c r="AA6">
+        <v>13</v>
+      </c>
+      <c r="AB6">
+        <v>1</v>
+      </c>
+      <c r="AC6" s="2">
+        <f t="shared" ref="AC6:AC38" si="0">AC5+(($AE$2)*(AB6-AC5))</f>
+        <v>0.42490000000000006</v>
+      </c>
+      <c r="AF6">
+        <v>3</v>
+      </c>
+      <c r="AG6">
+        <f>AF6*(1-((1-AE2)/2))</f>
+        <v>1.6500000000000001</v>
+      </c>
+    </row>
+    <row r="7" spans="2:33" x14ac:dyDescent="0.25">
+      <c r="B7" s="7">
         <v>44669</v>
       </c>
       <c r="C7" s="2">
@@ -23012,9 +23060,29 @@
       <c r="N7" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B8" s="9">
+      <c r="V7">
+        <v>22</v>
+      </c>
+      <c r="W7">
+        <v>1</v>
+      </c>
+      <c r="X7" s="2">
+        <f t="shared" ref="X7:X38" si="1">($AE$2*W7)+((1-$AE$2)*X6)</f>
+        <v>2.6200000000000006</v>
+      </c>
+      <c r="AA7">
+        <v>22</v>
+      </c>
+      <c r="AB7">
+        <v>1</v>
+      </c>
+      <c r="AC7" s="2">
+        <f t="shared" si="0"/>
+        <v>0.48241000000000006</v>
+      </c>
+    </row>
+    <row r="8" spans="2:33" x14ac:dyDescent="0.25">
+      <c r="B8" s="7">
         <v>44699</v>
       </c>
       <c r="C8" s="2">
@@ -23053,9 +23121,29 @@
       <c r="N8" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B9" s="9">
+      <c r="V8">
+        <v>49</v>
+      </c>
+      <c r="W8">
+        <v>1</v>
+      </c>
+      <c r="X8" s="2">
+        <f t="shared" si="1"/>
+        <v>2.4580000000000006</v>
+      </c>
+      <c r="AA8">
+        <v>49</v>
+      </c>
+      <c r="AB8">
+        <v>1</v>
+      </c>
+      <c r="AC8" s="2">
+        <f t="shared" si="0"/>
+        <v>0.53416900000000012</v>
+      </c>
+    </row>
+    <row r="9" spans="2:33" x14ac:dyDescent="0.25">
+      <c r="B9" s="7">
         <v>44730</v>
       </c>
       <c r="C9" s="2">
@@ -23094,9 +23182,29 @@
       <c r="N9" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B10" s="9">
+      <c r="V9">
+        <v>28</v>
+      </c>
+      <c r="W9">
+        <v>1</v>
+      </c>
+      <c r="X9" s="2">
+        <f t="shared" si="1"/>
+        <v>2.3122000000000007</v>
+      </c>
+      <c r="AA9">
+        <v>28</v>
+      </c>
+      <c r="AB9">
+        <v>1</v>
+      </c>
+      <c r="AC9" s="2">
+        <f t="shared" si="0"/>
+        <v>0.5807521000000001</v>
+      </c>
+    </row>
+    <row r="10" spans="2:33" x14ac:dyDescent="0.25">
+      <c r="B10" s="7">
         <v>44760</v>
       </c>
       <c r="C10" s="2">
@@ -23135,9 +23243,29 @@
       <c r="N10" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B11" s="9">
+      <c r="V10">
+        <v>15</v>
+      </c>
+      <c r="W10">
+        <v>1</v>
+      </c>
+      <c r="X10" s="2">
+        <f t="shared" si="1"/>
+        <v>2.1809800000000008</v>
+      </c>
+      <c r="AA10">
+        <v>15</v>
+      </c>
+      <c r="AB10">
+        <v>1</v>
+      </c>
+      <c r="AC10" s="2">
+        <f t="shared" si="0"/>
+        <v>0.62267689000000015</v>
+      </c>
+    </row>
+    <row r="11" spans="2:33" x14ac:dyDescent="0.25">
+      <c r="B11" s="7">
         <v>44791</v>
       </c>
       <c r="C11" s="2">
@@ -23176,9 +23304,29 @@
       <c r="N11" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B12" s="9">
+      <c r="V11">
+        <v>7</v>
+      </c>
+      <c r="W11">
+        <v>1</v>
+      </c>
+      <c r="X11" s="2">
+        <f t="shared" si="1"/>
+        <v>2.0628820000000005</v>
+      </c>
+      <c r="AA11">
+        <v>7</v>
+      </c>
+      <c r="AB11">
+        <v>1</v>
+      </c>
+      <c r="AC11" s="2">
+        <f t="shared" si="0"/>
+        <v>0.66040920100000011</v>
+      </c>
+    </row>
+    <row r="12" spans="2:33" x14ac:dyDescent="0.25">
+      <c r="B12" s="7">
         <v>44822</v>
       </c>
       <c r="C12" s="2">
@@ -23217,9 +23365,29 @@
       <c r="N12" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B13" s="9">
+      <c r="V12">
+        <v>13</v>
+      </c>
+      <c r="W12">
+        <v>1</v>
+      </c>
+      <c r="X12" s="2">
+        <f t="shared" si="1"/>
+        <v>1.9565938000000007</v>
+      </c>
+      <c r="AA12">
+        <v>13</v>
+      </c>
+      <c r="AB12">
+        <v>1</v>
+      </c>
+      <c r="AC12" s="2">
+        <f t="shared" si="0"/>
+        <v>0.69436828090000013</v>
+      </c>
+    </row>
+    <row r="13" spans="2:33" x14ac:dyDescent="0.25">
+      <c r="B13" s="7">
         <v>44852</v>
       </c>
       <c r="C13" s="2">
@@ -23258,9 +23426,29 @@
       <c r="N13" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B14" s="9">
+      <c r="V13">
+        <v>16</v>
+      </c>
+      <c r="W13">
+        <v>1</v>
+      </c>
+      <c r="X13" s="2">
+        <f t="shared" si="1"/>
+        <v>1.8609344200000009</v>
+      </c>
+      <c r="AA13">
+        <v>16</v>
+      </c>
+      <c r="AB13">
+        <v>1</v>
+      </c>
+      <c r="AC13" s="2">
+        <f t="shared" si="0"/>
+        <v>0.72493145281000015</v>
+      </c>
+    </row>
+    <row r="14" spans="2:33" x14ac:dyDescent="0.25">
+      <c r="B14" s="7">
         <v>44883</v>
       </c>
       <c r="C14" s="2">
@@ -23299,9 +23487,29 @@
       <c r="N14" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B15" s="9">
+      <c r="V14">
+        <v>29</v>
+      </c>
+      <c r="W14">
+        <v>1</v>
+      </c>
+      <c r="X14" s="2">
+        <f t="shared" si="1"/>
+        <v>1.774840978000001</v>
+      </c>
+      <c r="AA14">
+        <v>29</v>
+      </c>
+      <c r="AB14">
+        <v>1</v>
+      </c>
+      <c r="AC14" s="2">
+        <f t="shared" si="0"/>
+        <v>0.75243830752900009</v>
+      </c>
+    </row>
+    <row r="15" spans="2:33" x14ac:dyDescent="0.25">
+      <c r="B15" s="7">
         <v>44913</v>
       </c>
       <c r="C15" s="2">
@@ -23340,9 +23548,29 @@
       <c r="N15" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B16" s="9">
+      <c r="V15">
+        <v>22</v>
+      </c>
+      <c r="W15">
+        <v>1</v>
+      </c>
+      <c r="X15" s="2">
+        <f t="shared" si="1"/>
+        <v>1.697356880200001</v>
+      </c>
+      <c r="AA15">
+        <v>22</v>
+      </c>
+      <c r="AB15">
+        <v>1</v>
+      </c>
+      <c r="AC15" s="2">
+        <f t="shared" si="0"/>
+        <v>0.7771944767761001</v>
+      </c>
+    </row>
+    <row r="16" spans="2:33" x14ac:dyDescent="0.25">
+      <c r="B16" s="7">
         <v>44580</v>
       </c>
       <c r="C16" s="2">
@@ -23381,9 +23609,29 @@
       <c r="N16" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="17" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B17" s="9">
+      <c r="V16">
+        <v>6</v>
+      </c>
+      <c r="W16">
+        <v>1</v>
+      </c>
+      <c r="X16" s="2">
+        <f t="shared" si="1"/>
+        <v>1.627621192180001</v>
+      </c>
+      <c r="AA16">
+        <v>6</v>
+      </c>
+      <c r="AB16">
+        <v>1</v>
+      </c>
+      <c r="AC16" s="2">
+        <f t="shared" si="0"/>
+        <v>0.79947502909849011</v>
+      </c>
+    </row>
+    <row r="17" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="B17" s="7">
         <v>44611</v>
       </c>
       <c r="C17" s="2">
@@ -23422,9 +23670,29 @@
       <c r="N17" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B18" s="9">
+      <c r="V17">
+        <v>2</v>
+      </c>
+      <c r="W17">
+        <v>1</v>
+      </c>
+      <c r="X17" s="2">
+        <f t="shared" si="1"/>
+        <v>1.5648590729620011</v>
+      </c>
+      <c r="AA17">
+        <v>2</v>
+      </c>
+      <c r="AB17">
+        <v>1</v>
+      </c>
+      <c r="AC17" s="2">
+        <f t="shared" si="0"/>
+        <v>0.81952752618864111</v>
+      </c>
+    </row>
+    <row r="18" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="B18" s="7">
         <v>44639</v>
       </c>
       <c r="C18" s="2">
@@ -23463,9 +23731,29 @@
       <c r="N18" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="19" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B19" s="9">
+      <c r="V18">
+        <v>38</v>
+      </c>
+      <c r="W18">
+        <v>1</v>
+      </c>
+      <c r="X18" s="2">
+        <f t="shared" si="1"/>
+        <v>1.508373165665801</v>
+      </c>
+      <c r="AA18">
+        <v>38</v>
+      </c>
+      <c r="AB18">
+        <v>1</v>
+      </c>
+      <c r="AC18" s="2">
+        <f t="shared" si="0"/>
+        <v>0.83757477356977694</v>
+      </c>
+    </row>
+    <row r="19" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="B19" s="7">
         <v>44670</v>
       </c>
       <c r="C19" s="2">
@@ -23504,9 +23792,29 @@
       <c r="N19" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="20" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B20" s="9">
+      <c r="V19">
+        <v>45</v>
+      </c>
+      <c r="W19">
+        <v>1</v>
+      </c>
+      <c r="X19" s="2">
+        <f t="shared" si="1"/>
+        <v>1.457535849099221</v>
+      </c>
+      <c r="AA19">
+        <v>45</v>
+      </c>
+      <c r="AB19">
+        <v>1</v>
+      </c>
+      <c r="AC19" s="2">
+        <f t="shared" si="0"/>
+        <v>0.85381729621279923</v>
+      </c>
+    </row>
+    <row r="20" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="B20" s="7">
         <v>44700</v>
       </c>
       <c r="C20" s="2">
@@ -23545,9 +23853,29 @@
       <c r="N20" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="21" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B21" s="9">
+      <c r="V20">
+        <v>18</v>
+      </c>
+      <c r="W20">
+        <v>1</v>
+      </c>
+      <c r="X20" s="2">
+        <f t="shared" si="1"/>
+        <v>1.411782264189299</v>
+      </c>
+      <c r="AA20">
+        <v>18</v>
+      </c>
+      <c r="AB20">
+        <v>1</v>
+      </c>
+      <c r="AC20" s="2">
+        <f t="shared" si="0"/>
+        <v>0.86843556659151933</v>
+      </c>
+    </row>
+    <row r="21" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="B21" s="7">
         <v>44731</v>
       </c>
       <c r="C21" s="2">
@@ -23586,9 +23914,29 @@
       <c r="N21" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="22" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B22" s="9">
+      <c r="V21">
+        <v>1</v>
+      </c>
+      <c r="W21">
+        <v>1</v>
+      </c>
+      <c r="X21" s="2">
+        <f t="shared" si="1"/>
+        <v>1.3706040377703692</v>
+      </c>
+      <c r="AA21">
+        <v>1</v>
+      </c>
+      <c r="AB21">
+        <v>1</v>
+      </c>
+      <c r="AC21" s="2">
+        <f t="shared" si="0"/>
+        <v>0.88159200993236742</v>
+      </c>
+    </row>
+    <row r="22" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="B22" s="7">
         <v>44761</v>
       </c>
       <c r="C22" s="2">
@@ -23627,9 +23975,29 @@
       <c r="N22" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="23" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B23" s="9">
+      <c r="V22">
+        <v>37</v>
+      </c>
+      <c r="W22">
+        <v>1</v>
+      </c>
+      <c r="X22" s="2">
+        <f t="shared" si="1"/>
+        <v>1.3335436339933324</v>
+      </c>
+      <c r="AA22">
+        <v>37</v>
+      </c>
+      <c r="AB22">
+        <v>1</v>
+      </c>
+      <c r="AC22" s="2">
+        <f t="shared" si="0"/>
+        <v>0.89343280893913068</v>
+      </c>
+    </row>
+    <row r="23" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="B23" s="7">
         <v>44792</v>
       </c>
       <c r="C23" s="2">
@@ -23668,9 +24036,29 @@
       <c r="N23" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="24" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B24" s="9">
+      <c r="V23">
+        <v>45</v>
+      </c>
+      <c r="W23">
+        <v>1</v>
+      </c>
+      <c r="X23" s="2">
+        <f t="shared" si="1"/>
+        <v>1.3001892705939992</v>
+      </c>
+      <c r="AA23">
+        <v>45</v>
+      </c>
+      <c r="AB23">
+        <v>1</v>
+      </c>
+      <c r="AC23" s="2">
+        <f t="shared" si="0"/>
+        <v>0.90408952804521758</v>
+      </c>
+    </row>
+    <row r="24" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="B24" s="7">
         <v>44823</v>
       </c>
       <c r="C24" s="2">
@@ -23709,9 +24097,29 @@
       <c r="N24" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="25" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B25" s="9">
+      <c r="V24">
+        <v>12</v>
+      </c>
+      <c r="W24">
+        <v>1</v>
+      </c>
+      <c r="X24" s="2">
+        <f>($AE$2*W24)+((1-$AE$2)*X23)</f>
+        <v>1.2701703435345995</v>
+      </c>
+      <c r="AA24">
+        <v>12</v>
+      </c>
+      <c r="AB24">
+        <v>1</v>
+      </c>
+      <c r="AC24" s="2">
+        <f t="shared" si="0"/>
+        <v>0.91368057524069579</v>
+      </c>
+    </row>
+    <row r="25" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="B25" s="7">
         <v>44853</v>
       </c>
       <c r="C25" s="2">
@@ -23750,9 +24158,29 @@
       <c r="N25" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="26" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B26" s="9">
+      <c r="V25">
+        <v>22</v>
+      </c>
+      <c r="W25">
+        <v>1</v>
+      </c>
+      <c r="X25" s="2">
+        <f t="shared" si="1"/>
+        <v>1.2431533091811395</v>
+      </c>
+      <c r="AA25">
+        <v>22</v>
+      </c>
+      <c r="AB25">
+        <v>1</v>
+      </c>
+      <c r="AC25" s="2">
+        <f t="shared" si="0"/>
+        <v>0.92231251771662626</v>
+      </c>
+    </row>
+    <row r="26" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="B26" s="7">
         <v>44884</v>
       </c>
       <c r="C26" s="2">
@@ -23791,9 +24219,29 @@
       <c r="N26" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="27" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B27" s="9">
+      <c r="V26">
+        <v>16</v>
+      </c>
+      <c r="W26">
+        <v>1</v>
+      </c>
+      <c r="X26" s="2">
+        <f t="shared" si="1"/>
+        <v>1.2188379782630256</v>
+      </c>
+      <c r="AA26">
+        <v>16</v>
+      </c>
+      <c r="AB26">
+        <v>1</v>
+      </c>
+      <c r="AC26" s="2">
+        <f t="shared" si="0"/>
+        <v>0.93008126594496365</v>
+      </c>
+    </row>
+    <row r="27" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="B27" s="7">
         <v>44914</v>
       </c>
       <c r="C27" s="2">
@@ -23832,9 +24280,29 @@
       <c r="N27" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="28" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B28" s="9">
+      <c r="V27">
+        <v>18</v>
+      </c>
+      <c r="W27">
+        <v>1</v>
+      </c>
+      <c r="X27" s="2">
+        <f t="shared" si="1"/>
+        <v>1.1969541804367232</v>
+      </c>
+      <c r="AA27">
+        <v>18</v>
+      </c>
+      <c r="AB27">
+        <v>1</v>
+      </c>
+      <c r="AC27" s="2">
+        <f t="shared" si="0"/>
+        <v>0.93707313935046732</v>
+      </c>
+    </row>
+    <row r="28" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="B28" s="7">
         <v>44581</v>
       </c>
       <c r="C28" s="2">
@@ -23873,9 +24341,29 @@
       <c r="N28" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="29" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B29" s="9">
+      <c r="V28">
+        <v>27</v>
+      </c>
+      <c r="W28">
+        <v>1</v>
+      </c>
+      <c r="X28" s="2">
+        <f>($AE$2*W28)+((1-$AE$2)*X27)</f>
+        <v>1.1772587623930511</v>
+      </c>
+      <c r="AA28">
+        <v>27</v>
+      </c>
+      <c r="AB28">
+        <v>1</v>
+      </c>
+      <c r="AC28" s="2">
+        <f t="shared" si="0"/>
+        <v>0.94336582541542058</v>
+      </c>
+    </row>
+    <row r="29" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="B29" s="7">
         <v>44612</v>
       </c>
       <c r="C29" s="2">
@@ -23914,9 +24402,29 @@
       <c r="N29" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="30" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B30" s="9">
+      <c r="V29">
+        <v>14</v>
+      </c>
+      <c r="W29">
+        <v>1</v>
+      </c>
+      <c r="X29" s="2">
+        <f t="shared" si="1"/>
+        <v>1.1595328861537462</v>
+      </c>
+      <c r="AA29">
+        <v>14</v>
+      </c>
+      <c r="AB29">
+        <v>1</v>
+      </c>
+      <c r="AC29" s="2">
+        <f t="shared" si="0"/>
+        <v>0.94902924287387846</v>
+      </c>
+    </row>
+    <row r="30" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="B30" s="7">
         <v>44640</v>
       </c>
       <c r="C30" s="2">
@@ -23955,9 +24463,29 @@
       <c r="N30" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="31" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B31" s="9">
+      <c r="V30">
+        <v>4</v>
+      </c>
+      <c r="W30">
+        <v>1</v>
+      </c>
+      <c r="X30" s="2">
+        <f t="shared" si="1"/>
+        <v>1.1435795975383716</v>
+      </c>
+      <c r="AA30">
+        <v>4</v>
+      </c>
+      <c r="AB30">
+        <v>1</v>
+      </c>
+      <c r="AC30" s="2">
+        <f t="shared" si="0"/>
+        <v>0.95412631858649066</v>
+      </c>
+    </row>
+    <row r="31" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="B31" s="7">
         <v>44671</v>
       </c>
       <c r="C31" s="2">
@@ -23996,9 +24524,29 @@
       <c r="N31" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="32" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B32" s="9">
+      <c r="V31">
+        <v>5</v>
+      </c>
+      <c r="W31">
+        <v>1</v>
+      </c>
+      <c r="X31" s="2">
+        <f t="shared" si="1"/>
+        <v>1.1292216377845345</v>
+      </c>
+      <c r="AA31">
+        <v>5</v>
+      </c>
+      <c r="AB31">
+        <v>1</v>
+      </c>
+      <c r="AC31" s="2">
+        <f t="shared" si="0"/>
+        <v>0.95871368672784163</v>
+      </c>
+    </row>
+    <row r="32" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="B32" s="7">
         <v>44701</v>
       </c>
       <c r="C32" s="2">
@@ -24037,9 +24585,29 @@
       <c r="N32" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="33" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B33" s="9">
+      <c r="V32">
+        <v>6</v>
+      </c>
+      <c r="W32">
+        <v>1</v>
+      </c>
+      <c r="X32" s="2">
+        <f t="shared" si="1"/>
+        <v>1.1162994740060812</v>
+      </c>
+      <c r="AA32">
+        <v>6</v>
+      </c>
+      <c r="AB32">
+        <v>1</v>
+      </c>
+      <c r="AC32" s="2">
+        <f t="shared" si="0"/>
+        <v>0.96284231805505749</v>
+      </c>
+    </row>
+    <row r="33" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="B33" s="7">
         <v>44732</v>
       </c>
       <c r="C33" s="2">
@@ -24078,9 +24646,29 @@
       <c r="N33" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="34" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B34" s="9">
+      <c r="V33">
+        <v>1</v>
+      </c>
+      <c r="W33">
+        <v>1</v>
+      </c>
+      <c r="X33" s="2">
+        <f t="shared" si="1"/>
+        <v>1.1046695266054731</v>
+      </c>
+      <c r="AA33">
+        <v>1</v>
+      </c>
+      <c r="AB33">
+        <v>1</v>
+      </c>
+      <c r="AC33" s="2">
+        <f t="shared" si="0"/>
+        <v>0.96655808624955175</v>
+      </c>
+    </row>
+    <row r="34" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="B34" s="7">
         <v>44762</v>
       </c>
       <c r="C34" s="2">
@@ -24119,9 +24707,29 @@
       <c r="N34" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="35" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B35" s="9">
+      <c r="V34">
+        <v>28</v>
+      </c>
+      <c r="W34">
+        <v>1</v>
+      </c>
+      <c r="X34" s="2">
+        <f>($AE$2*W34)+((1-$AE$2)*X33)</f>
+        <v>1.0942025739449259</v>
+      </c>
+      <c r="AA34">
+        <v>28</v>
+      </c>
+      <c r="AB34">
+        <v>1</v>
+      </c>
+      <c r="AC34" s="2">
+        <f t="shared" si="0"/>
+        <v>0.96990227762459658</v>
+      </c>
+    </row>
+    <row r="35" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="B35" s="7">
         <v>44793</v>
       </c>
       <c r="C35" s="2">
@@ -24160,9 +24768,29 @@
       <c r="N35" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="36" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B36" s="9">
+      <c r="V35">
+        <v>0</v>
+      </c>
+      <c r="W35" s="11">
+        <v>1</v>
+      </c>
+      <c r="X35" s="2">
+        <f>($AE$2*W35)+((1-$AE$2)*X34)</f>
+        <v>1.0847823165504333</v>
+      </c>
+      <c r="AA35">
+        <v>0</v>
+      </c>
+      <c r="AB35">
+        <v>0</v>
+      </c>
+      <c r="AC35" s="2">
+        <f t="shared" si="0"/>
+        <v>0.87291204986213689</v>
+      </c>
+    </row>
+    <row r="36" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="B36" s="7">
         <v>44824</v>
       </c>
       <c r="C36" s="2">
@@ -24201,9 +24829,28 @@
       <c r="N36" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="37" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B37" s="9">
+      <c r="V36">
+        <v>0</v>
+      </c>
+      <c r="W36" s="11">
+        <v>1</v>
+      </c>
+      <c r="X36" s="2">
+        <v>1.0847823165504333</v>
+      </c>
+      <c r="AA36">
+        <v>0</v>
+      </c>
+      <c r="AB36">
+        <v>2</v>
+      </c>
+      <c r="AC36" s="2">
+        <f t="shared" si="0"/>
+        <v>0.98562084487592316</v>
+      </c>
+    </row>
+    <row r="37" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="B37" s="7">
         <v>44854</v>
       </c>
       <c r="C37" s="2">
@@ -24242,9 +24889,28 @@
       <c r="N37" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="38" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B38" s="9">
+      <c r="V37">
+        <v>41</v>
+      </c>
+      <c r="W37" s="11">
+        <v>1</v>
+      </c>
+      <c r="X37" s="2">
+        <v>1.0847823165504333</v>
+      </c>
+      <c r="AA37">
+        <v>41</v>
+      </c>
+      <c r="AB37">
+        <v>3</v>
+      </c>
+      <c r="AC37" s="2">
+        <f t="shared" si="0"/>
+        <v>1.1870587603883309</v>
+      </c>
+    </row>
+    <row r="38" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="B38" s="7">
         <v>44885</v>
       </c>
       <c r="C38" s="2">
@@ -24281,6 +24947,31 @@
         <v>1.000189</v>
       </c>
       <c r="N38" s="2">
+        <v>1</v>
+      </c>
+      <c r="V38">
+        <v>60</v>
+      </c>
+      <c r="W38">
+        <v>3</v>
+      </c>
+      <c r="X38" s="2">
+        <f>($AE$2*W38)+((1-$AE$2)*X37)</f>
+        <v>1.2763040848953899</v>
+      </c>
+      <c r="AA38">
+        <v>60</v>
+      </c>
+      <c r="AB38">
+        <v>1</v>
+      </c>
+      <c r="AC38" s="2">
+        <f t="shared" si="0"/>
+        <v>1.1683528843494979</v>
+      </c>
+    </row>
+    <row r="39" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="W39">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Finished erratic item. Begining intermittent item
</commit_message>
<xml_diff>
--- a/bip1271_data.xlsx
+++ b/bip1271_data.xlsx
@@ -22740,8 +22740,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:AG39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="S37" sqref="S37"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="W38" sqref="W38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -24836,7 +24836,7 @@
         <v>1</v>
       </c>
       <c r="X36" s="2">
-        <v>1.0847823165504333</v>
+        <v>1.08478231655043</v>
       </c>
       <c r="AA36">
         <v>0</v>
@@ -24896,7 +24896,7 @@
         <v>1</v>
       </c>
       <c r="X37" s="2">
-        <v>1.0847823165504333</v>
+        <v>1.08478231655043</v>
       </c>
       <c r="AA37">
         <v>41</v>
@@ -24957,7 +24957,7 @@
       </c>
       <c r="X38" s="2">
         <f>($AE$2*W38)+((1-$AE$2)*X37)</f>
-        <v>1.2763040848953899</v>
+        <v>1.276304084895387</v>
       </c>
       <c r="AA38">
         <v>60</v>

</xml_diff>

<commit_message>
Added aggregation reuslts for the first item
</commit_message>
<xml_diff>
--- a/bip1271_data.xlsx
+++ b/bip1271_data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" activeTab="5"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,19 +18,21 @@
     <sheet name="0.5" sheetId="3" r:id="rId4"/>
     <sheet name="optimal" sheetId="6" r:id="rId5"/>
     <sheet name="interdemand inter." sheetId="8" r:id="rId6"/>
+    <sheet name="Agregate-Disaggregate" sheetId="9" r:id="rId7"/>
+    <sheet name="Sheet3" sheetId="10" r:id="rId8"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId7"/>
-    <externalReference r:id="rId8"/>
     <externalReference r:id="rId9"/>
     <externalReference r:id="rId10"/>
+    <externalReference r:id="rId11"/>
+    <externalReference r:id="rId12"/>
   </externalReferences>
   <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="437" uniqueCount="77">
   <si>
     <t>X</t>
   </si>
@@ -252,6 +254,15 @@
   </si>
   <si>
     <t>SBJ (0.15)</t>
+  </si>
+  <si>
+    <t>Aggregation</t>
+  </si>
+  <si>
+    <t>ADIDA</t>
+  </si>
+  <si>
+    <t>MAPA</t>
   </si>
 </sst>
 </file>
@@ -7832,6 +7843,1557 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Agregation of second level</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Agregate-Disaggregate'!$A$2:$A$37</c:f>
+              <c:strCache>
+                <c:ptCount val="36"/>
+                <c:pt idx="0">
+                  <c:v>Dec-17</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Jan-18</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Feb-18</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Mar-18</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Apr-18</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>May-18</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Jun-18</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Jul-18</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Aug-18</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Sep-18</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Oct-18</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Nov-18</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>Dec-18</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>Jan-19</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>Feb-19</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>Mar-19</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>Apr-19</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>May-19</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>Jun-19</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>Jul-19</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>Aug-19</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>Sep-19</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>Oct-19</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>Nov-19</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>Dec-19</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>Jan-20</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>Feb-20</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>Mar-20</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>Apr-20</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>May-20</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>Jun-20</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>Jul-20</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>Aug-20</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>Sep-20</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>Oct-20</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>Nov-20</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Agregate-Disaggregate'!$C$2:$C$37</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="36"/>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>71</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>43</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>63</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>57</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>101</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-DB4F-40CF-8FE5-274EAA183582}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:axId val="474635240"/>
+        <c:axId val="474627040"/>
+      </c:barChart>
+      <c:lineChart>
+        <c:grouping val="stacked"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Agregate-Disaggregate'!$A$2:$A$37</c:f>
+              <c:strCache>
+                <c:ptCount val="36"/>
+                <c:pt idx="0">
+                  <c:v>Dec-17</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Jan-18</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Feb-18</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Mar-18</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Apr-18</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>May-18</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Jun-18</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Jul-18</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Aug-18</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Sep-18</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Oct-18</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Nov-18</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>Dec-18</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>Jan-19</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>Feb-19</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>Mar-19</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>Apr-19</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>May-19</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>Jun-19</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>Jul-19</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>Aug-19</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>Sep-19</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>Oct-19</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>Nov-19</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>Dec-19</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>Jan-20</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>Feb-20</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>Mar-20</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>Apr-20</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>May-20</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>Jun-20</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>Jul-20</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>Aug-20</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>Sep-20</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>Oct-20</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>Nov-20</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Agregate-Disaggregate'!$B$2:$B$37</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="36"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>49</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>41</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>60</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-DB4F-40CF-8FE5-274EAA183582}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="474635240"/>
+        <c:axId val="474627040"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="474635240"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="474627040"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="474627040"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="474635240"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Agregate-Disaggregate'!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>BIP001271</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Agregate-Disaggregate'!$A$2:$A$37</c:f>
+              <c:strCache>
+                <c:ptCount val="36"/>
+                <c:pt idx="0">
+                  <c:v>Dec-17</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Jan-18</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Feb-18</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Mar-18</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Apr-18</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>May-18</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Jun-18</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Jul-18</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Aug-18</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Sep-18</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Oct-18</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Nov-18</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>Dec-18</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>Jan-19</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>Feb-19</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>Mar-19</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>Apr-19</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>May-19</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>Jun-19</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>Jul-19</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>Aug-19</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>Sep-19</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>Oct-19</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>Nov-19</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>Dec-19</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>Jan-20</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>Feb-20</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>Mar-20</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>Apr-20</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>May-20</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>Jun-20</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>Jul-20</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>Aug-20</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>Sep-20</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>Oct-20</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>Nov-20</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Agregate-Disaggregate'!$B$2:$B$37</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="36"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>49</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>41</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>60</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-10B7-4DC0-B208-3894CC7A5056}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Agregate-Disaggregate'!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>ADIDA</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Agregate-Disaggregate'!$A$2:$A$37</c:f>
+              <c:strCache>
+                <c:ptCount val="36"/>
+                <c:pt idx="0">
+                  <c:v>Dec-17</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Jan-18</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Feb-18</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Mar-18</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Apr-18</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>May-18</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Jun-18</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Jul-18</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Aug-18</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Sep-18</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Oct-18</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Nov-18</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>Dec-18</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>Jan-19</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>Feb-19</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>Mar-19</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>Apr-19</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>May-19</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>Jun-19</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>Jul-19</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>Aug-19</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>Sep-19</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>Oct-19</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>Nov-19</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>Dec-19</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>Jan-20</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>Feb-20</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>Mar-20</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>Apr-20</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>May-20</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>Jun-20</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>Jul-20</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>Aug-20</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>Sep-20</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>Oct-20</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>Nov-20</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Agregate-Disaggregate'!$D$2:$D$37</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="36"/>
+                <c:pt idx="2">
+                  <c:v>6.1503969999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6.1503969999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8.4141709999999996</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8.4141709999999996</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>15.757759999999999</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>15.757759999999999</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>17.314620000000001</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>17.314620000000001</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>15.33146</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>15.33146</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>17.275010000000002</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>17.275010000000002</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>16.387080000000001</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>16.387080000000001</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>17.366630000000001</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>17.366630000000001</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>21.198509999999999</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>21.198509999999999</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>20.602440000000001</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>20.602440000000001</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>22.743649999999999</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>22.743649999999999</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>21.728660000000001</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>21.728660000000001</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>21.93779</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>21.93779</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>18.430060000000001</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>18.430060000000001</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>14.92442</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>14.92442</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>14.80935</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>14.80935</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>14.80935</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>14.80935</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-10B7-4DC0-B208-3894CC7A5056}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="529212048"/>
+        <c:axId val="529213032"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="529212048"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="529213032"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="529213032"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="529212048"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
       <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
@@ -8060,6 +9622,86 @@
 </file>
 
 <file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors7.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -10614,6 +12256,1012 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style7.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -10789,6 +13437,71 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>533400</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>604836</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>590549</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -14230,8 +16943,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V65"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="T41" sqref="T41"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -21505,7 +24218,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:AG39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
@@ -23750,4 +26463,878 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E37"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C37"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D1" t="s">
+        <v>75</v>
+      </c>
+      <c r="E1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3">
+        <v>10</v>
+      </c>
+      <c r="C3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4">
+        <v>16</v>
+      </c>
+      <c r="D4">
+        <v>6.1503969999999999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5">
+        <v>13</v>
+      </c>
+      <c r="C5">
+        <v>29</v>
+      </c>
+      <c r="D5">
+        <v>6.1503969999999999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6">
+        <v>22</v>
+      </c>
+      <c r="D6">
+        <v>8.4141709999999996</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7">
+        <v>49</v>
+      </c>
+      <c r="C7">
+        <v>71</v>
+      </c>
+      <c r="D7">
+        <v>8.4141709999999996</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8">
+        <v>28</v>
+      </c>
+      <c r="D8">
+        <v>15.757759999999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9">
+        <v>15</v>
+      </c>
+      <c r="C9">
+        <v>43</v>
+      </c>
+      <c r="D9">
+        <v>15.757759999999999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10">
+        <v>7</v>
+      </c>
+      <c r="D10">
+        <v>17.314620000000001</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11">
+        <v>13</v>
+      </c>
+      <c r="C11">
+        <v>20</v>
+      </c>
+      <c r="D11">
+        <v>17.314620000000001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12">
+        <v>16</v>
+      </c>
+      <c r="D12">
+        <v>15.33146</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13">
+        <v>29</v>
+      </c>
+      <c r="C13">
+        <v>45</v>
+      </c>
+      <c r="D13">
+        <v>15.33146</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>22</v>
+      </c>
+      <c r="B14">
+        <v>22</v>
+      </c>
+      <c r="D14">
+        <v>17.275010000000002</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>23</v>
+      </c>
+      <c r="B15">
+        <v>6</v>
+      </c>
+      <c r="C15">
+        <v>28</v>
+      </c>
+      <c r="D15">
+        <v>17.275010000000002</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>24</v>
+      </c>
+      <c r="B16">
+        <v>2</v>
+      </c>
+      <c r="D16">
+        <v>16.387080000000001</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>25</v>
+      </c>
+      <c r="B17">
+        <v>38</v>
+      </c>
+      <c r="C17">
+        <v>40</v>
+      </c>
+      <c r="D17">
+        <v>16.387080000000001</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>26</v>
+      </c>
+      <c r="B18">
+        <v>45</v>
+      </c>
+      <c r="D18">
+        <v>17.366630000000001</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>27</v>
+      </c>
+      <c r="B19">
+        <v>18</v>
+      </c>
+      <c r="C19">
+        <v>63</v>
+      </c>
+      <c r="D19">
+        <v>17.366630000000001</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>28</v>
+      </c>
+      <c r="B20">
+        <v>1</v>
+      </c>
+      <c r="D20">
+        <v>21.198509999999999</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>29</v>
+      </c>
+      <c r="B21">
+        <v>37</v>
+      </c>
+      <c r="C21">
+        <v>38</v>
+      </c>
+      <c r="D21">
+        <v>21.198509999999999</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>30</v>
+      </c>
+      <c r="B22">
+        <v>45</v>
+      </c>
+      <c r="D22">
+        <v>20.602440000000001</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>31</v>
+      </c>
+      <c r="B23">
+        <v>12</v>
+      </c>
+      <c r="C23">
+        <v>57</v>
+      </c>
+      <c r="D23">
+        <v>20.602440000000001</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>32</v>
+      </c>
+      <c r="B24">
+        <v>22</v>
+      </c>
+      <c r="D24">
+        <v>22.743649999999999</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>33</v>
+      </c>
+      <c r="B25">
+        <v>16</v>
+      </c>
+      <c r="C25">
+        <v>38</v>
+      </c>
+      <c r="D25">
+        <v>22.743649999999999</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>34</v>
+      </c>
+      <c r="B26">
+        <v>18</v>
+      </c>
+      <c r="D26">
+        <v>21.728660000000001</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>35</v>
+      </c>
+      <c r="B27">
+        <v>27</v>
+      </c>
+      <c r="C27">
+        <v>45</v>
+      </c>
+      <c r="D27">
+        <v>21.728660000000001</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>36</v>
+      </c>
+      <c r="B28">
+        <v>14</v>
+      </c>
+      <c r="D28">
+        <v>21.93779</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>37</v>
+      </c>
+      <c r="B29">
+        <v>4</v>
+      </c>
+      <c r="C29">
+        <v>18</v>
+      </c>
+      <c r="D29">
+        <v>21.93779</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>38</v>
+      </c>
+      <c r="B30">
+        <v>5</v>
+      </c>
+      <c r="D30">
+        <v>18.430060000000001</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>39</v>
+      </c>
+      <c r="B31">
+        <v>6</v>
+      </c>
+      <c r="C31">
+        <v>11</v>
+      </c>
+      <c r="D31">
+        <v>18.430060000000001</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>40</v>
+      </c>
+      <c r="B32">
+        <v>1</v>
+      </c>
+      <c r="D32">
+        <v>14.92442</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>41</v>
+      </c>
+      <c r="B33">
+        <v>28</v>
+      </c>
+      <c r="C33">
+        <v>29</v>
+      </c>
+      <c r="D33">
+        <v>14.92442</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>42</v>
+      </c>
+      <c r="B34">
+        <v>0</v>
+      </c>
+      <c r="D34">
+        <v>14.80935</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>43</v>
+      </c>
+      <c r="B35">
+        <v>0</v>
+      </c>
+      <c r="C35">
+        <v>0</v>
+      </c>
+      <c r="D35">
+        <v>14.80935</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>44</v>
+      </c>
+      <c r="B36">
+        <v>41</v>
+      </c>
+      <c r="D36">
+        <v>14.80935</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>45</v>
+      </c>
+      <c r="B37">
+        <v>60</v>
+      </c>
+      <c r="C37">
+        <v>101</v>
+      </c>
+      <c r="D37">
+        <v>14.80935</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{05C60535-1F16-4fd2-B633-F4F36F0B64E0}">
+      <x14:sparklineGroups xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+        <x14:sparklineGroup displayEmptyCellsAs="gap">
+          <x14:colorSeries rgb="FF376092"/>
+          <x14:colorNegative rgb="FFD00000"/>
+          <x14:colorAxis rgb="FF000000"/>
+          <x14:colorMarkers rgb="FFD00000"/>
+          <x14:colorFirst rgb="FFD00000"/>
+          <x14:colorLast rgb="FFD00000"/>
+          <x14:colorHigh rgb="FFD00000"/>
+          <x14:colorLow rgb="FFD00000"/>
+          <x14:sparklines>
+            <x14:sparkline>
+              <xm:f>'Agregate-Disaggregate'!C2:C37</xm:f>
+              <xm:sqref>F9</xm:sqref>
+            </x14:sparkline>
+          </x14:sparklines>
+        </x14:sparklineGroup>
+      </x14:sparklineGroups>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C37"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:C37"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3">
+        <v>10</v>
+      </c>
+      <c r="C3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5">
+        <v>13</v>
+      </c>
+      <c r="C5">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7">
+        <v>49</v>
+      </c>
+      <c r="C7">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9">
+        <v>15</v>
+      </c>
+      <c r="C9">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11">
+        <v>13</v>
+      </c>
+      <c r="C11">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13">
+        <v>29</v>
+      </c>
+      <c r="C13">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>22</v>
+      </c>
+      <c r="B14">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>23</v>
+      </c>
+      <c r="B15">
+        <v>6</v>
+      </c>
+      <c r="C15">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>24</v>
+      </c>
+      <c r="B16">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>25</v>
+      </c>
+      <c r="B17">
+        <v>38</v>
+      </c>
+      <c r="C17">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>26</v>
+      </c>
+      <c r="B18">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>27</v>
+      </c>
+      <c r="B19">
+        <v>18</v>
+      </c>
+      <c r="C19">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>28</v>
+      </c>
+      <c r="B20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>29</v>
+      </c>
+      <c r="B21">
+        <v>37</v>
+      </c>
+      <c r="C21">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>30</v>
+      </c>
+      <c r="B22">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>31</v>
+      </c>
+      <c r="B23">
+        <v>12</v>
+      </c>
+      <c r="C23">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>32</v>
+      </c>
+      <c r="B24">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>33</v>
+      </c>
+      <c r="B25">
+        <v>16</v>
+      </c>
+      <c r="C25">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>34</v>
+      </c>
+      <c r="B26">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>35</v>
+      </c>
+      <c r="B27">
+        <v>27</v>
+      </c>
+      <c r="C27">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>36</v>
+      </c>
+      <c r="B28">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>37</v>
+      </c>
+      <c r="B29">
+        <v>4</v>
+      </c>
+      <c r="C29">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>38</v>
+      </c>
+      <c r="B30">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>39</v>
+      </c>
+      <c r="B31">
+        <v>6</v>
+      </c>
+      <c r="C31">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>40</v>
+      </c>
+      <c r="B32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>41</v>
+      </c>
+      <c r="B33">
+        <v>28</v>
+      </c>
+      <c r="C33">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>42</v>
+      </c>
+      <c r="B34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>43</v>
+      </c>
+      <c r="B35">
+        <v>0</v>
+      </c>
+      <c r="C35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>44</v>
+      </c>
+      <c r="B36">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>45</v>
+      </c>
+      <c r="B37">
+        <v>60</v>
+      </c>
+      <c r="C37">
+        <v>101</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Chapter 4 finished. Added the modifications given by professor and the proposal assestment
</commit_message>
<xml_diff>
--- a/bip1271_data.xlsx
+++ b/bip1271_data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" activeTab="4"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="467" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="475" uniqueCount="80">
   <si>
     <t>X</t>
   </si>
@@ -232,24 +232,6 @@
     <t>t</t>
   </si>
   <si>
-    <t>SES (0.1)</t>
-  </si>
-  <si>
-    <t>SES (0.15)</t>
-  </si>
-  <si>
-    <t>Croston (0.1)</t>
-  </si>
-  <si>
-    <t>Croston (0.15)</t>
-  </si>
-  <si>
-    <t>SBA (0.1)</t>
-  </si>
-  <si>
-    <t>SBA (0.15)</t>
-  </si>
-  <si>
     <t>SBJ (0.1)</t>
   </si>
   <si>
@@ -284,6 +266,12 @@
   </si>
   <si>
     <t>Aggr. 9 level</t>
+  </si>
+  <si>
+    <t>SBA (0.5)</t>
+  </si>
+  <si>
+    <t>SBJ (0.0914)</t>
   </si>
 </sst>
 </file>
@@ -361,10 +349,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1934,7 +1922,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2564,7 +2551,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2671,7 +2657,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3298,7 +3283,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4142,7 +4126,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4775,7 +4758,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -11638,7 +11620,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -12534,7 +12515,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -12646,7 +12626,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -13315,7 +13294,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -13422,7 +13400,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -14073,7 +14050,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -14185,7 +14161,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -14827,7 +14802,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -26392,20 +26366,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z65"/>
+  <dimension ref="A1:AD65"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="Z19" sqref="Z19"/>
+    <sheetView tabSelected="1" topLeftCell="F2" workbookViewId="0">
+      <selection activeCell="AB5" sqref="AB5:AD13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="8" max="8" width="20.140625" customWidth="1"/>
     <col min="9" max="9" width="17" customWidth="1"/>
+    <col min="13" max="13" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="7.85546875" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="12.5703125" customWidth="1"/>
+    <col min="27" max="27" width="11.28515625" customWidth="1"/>
+    <col min="29" max="29" width="10.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -26413,7 +26391,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -26427,7 +26405,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -26459,7 +26437,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -26497,7 +26475,7 @@
         <v>2.1649449999999999</v>
       </c>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -26534,8 +26512,20 @@
       <c r="V5" s="2">
         <v>12.036384</v>
       </c>
+      <c r="Y5" t="s">
+        <v>68</v>
+      </c>
+      <c r="Z5" t="s">
+        <v>69</v>
+      </c>
+      <c r="AC5" t="s">
+        <v>66</v>
+      </c>
+      <c r="AD5" t="s">
+        <v>69</v>
+      </c>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>14</v>
       </c>
@@ -26572,8 +26562,26 @@
       <c r="V6" s="2">
         <v>15.774134</v>
       </c>
+      <c r="X6" t="s">
+        <v>55</v>
+      </c>
+      <c r="Y6" s="2">
+        <v>3.2121460000000002</v>
+      </c>
+      <c r="Z6" s="2">
+        <v>2.1843254999999999</v>
+      </c>
+      <c r="AB6" t="s">
+        <v>55</v>
+      </c>
+      <c r="AC6" s="2">
+        <v>1.840646</v>
+      </c>
+      <c r="AD6" s="2">
+        <v>2.1843254999999999</v>
+      </c>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>15</v>
       </c>
@@ -26618,30 +26626,66 @@
         <f>V6-V5</f>
         <v>3.7377500000000001</v>
       </c>
+      <c r="X7" t="s">
+        <v>56</v>
+      </c>
+      <c r="Y7" s="2">
+        <v>13.009081999999999</v>
+      </c>
+      <c r="Z7" s="2">
+        <v>12.744807</v>
+      </c>
+      <c r="AB7" t="s">
+        <v>56</v>
+      </c>
+      <c r="AC7" s="2">
+        <v>11.962090999999999</v>
+      </c>
+      <c r="AD7" s="2">
+        <v>12.744807</v>
+      </c>
     </row>
-    <row r="8" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>16</v>
       </c>
       <c r="B8">
         <v>28</v>
       </c>
-      <c r="K8" s="11" t="s">
+      <c r="K8" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="L8" s="11"/>
-      <c r="M8" s="11"/>
-      <c r="N8" s="11"/>
-      <c r="O8" s="11"/>
-      <c r="R8" s="11" t="s">
+      <c r="L8" s="10"/>
+      <c r="M8" s="10"/>
+      <c r="N8" s="10"/>
+      <c r="O8" s="10"/>
+      <c r="R8" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="S8" s="11"/>
-      <c r="T8" s="11"/>
-      <c r="U8" s="11"/>
-      <c r="V8" s="11"/>
+      <c r="S8" s="10"/>
+      <c r="T8" s="10"/>
+      <c r="U8" s="10"/>
+      <c r="V8" s="10"/>
+      <c r="X8" t="s">
+        <v>57</v>
+      </c>
+      <c r="Y8" s="2">
+        <v>16.492356999999998</v>
+      </c>
+      <c r="Z8" s="2">
+        <v>15.649894</v>
+      </c>
+      <c r="AB8" t="s">
+        <v>57</v>
+      </c>
+      <c r="AC8" s="2">
+        <v>15.5754</v>
+      </c>
+      <c r="AD8" s="2">
+        <v>15.649894</v>
+      </c>
     </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>17</v>
       </c>
@@ -26653,35 +26697,57 @@
       </c>
       <c r="L9" s="5"/>
       <c r="M9" s="5">
-        <f>(L6-M6)/M6</f>
-        <v>0.12053679712792387</v>
+        <f>(M6-L6)/L6</f>
+        <v>-0.10757058352467744</v>
       </c>
       <c r="N9" s="5">
-        <f>(L6-N6)/N6</f>
-        <v>0.12125110600575575</v>
+        <f>(N6-L6)/L6</f>
+        <v>-0.10813911830837769</v>
       </c>
       <c r="O9" s="5">
-        <f>(L6-O6)/O6</f>
-        <v>0.1211546412933215</v>
+        <f>(O6-L6)/L6</f>
+        <v>-0.1080623821469999</v>
       </c>
       <c r="R9" s="4" t="s">
         <v>51</v>
       </c>
       <c r="S9" s="5"/>
       <c r="T9" s="5">
-        <f>(S6-T6)/T6</f>
-        <v>8.2792442473829816E-2</v>
+        <f>(T6-S6)/S6</f>
+        <v>-7.6461969280720063E-2</v>
       </c>
       <c r="U9" s="5">
-        <f>(S6-U6)/U6</f>
-        <v>8.422801533115841E-2</v>
+        <f>(U6-S6)/S6</f>
+        <v>-7.7684780452230276E-2</v>
       </c>
       <c r="V9" s="5">
-        <f>(S6-V6)/V6</f>
-        <v>8.4516081833715909E-2</v>
+        <f>(V6-S6)/S6</f>
+        <v>-7.7929763559443824E-2</v>
+      </c>
+      <c r="X9" t="s">
+        <v>60</v>
+      </c>
+      <c r="Y9" s="2">
+        <f>Y8-Y7</f>
+        <v>3.483274999999999</v>
+      </c>
+      <c r="Z9" s="2">
+        <f>Z8-Z7</f>
+        <v>2.905087</v>
+      </c>
+      <c r="AB9" t="s">
+        <v>60</v>
+      </c>
+      <c r="AC9" s="2">
+        <f>AC8-AC7</f>
+        <v>3.613309000000001</v>
+      </c>
+      <c r="AD9" s="2">
+        <f>AD8-AD7</f>
+        <v>2.905087</v>
       </c>
     </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>18</v>
       </c>
@@ -26691,37 +26757,41 @@
       <c r="K10" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="L10" s="5">
-        <f>(M6-L6)/L6</f>
-        <v>-0.10757058352467744</v>
-      </c>
+      <c r="L10" s="5"/>
       <c r="M10" s="5"/>
       <c r="N10" s="5">
-        <f>(M6-N6)/N6</f>
-        <v>6.3747025502665215E-4</v>
+        <f>(N6-M6)/M6</f>
+        <v>-6.3706414558329879E-4</v>
       </c>
       <c r="O10" s="5">
-        <f>(M6-O6)/O6</f>
-        <v>5.5138230799848457E-4</v>
+        <f>(O6-M6)/M6</f>
+        <v>-5.5107845308913195E-4</v>
       </c>
       <c r="R10" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="S10" s="5">
-        <f>(T6-S6)/S6</f>
-        <v>-7.6461969280720063E-2</v>
-      </c>
+      <c r="S10" s="5"/>
       <c r="T10" s="5"/>
       <c r="U10" s="5">
-        <f>(T6-U6)/U6</f>
-        <v>1.3258061296113018E-3</v>
+        <f>(U6-T6)/T6</f>
+        <v>-1.3240506950838436E-3</v>
       </c>
       <c r="V10" s="5">
-        <f>(T6-V6)/V6</f>
-        <v>1.5918465000994504E-3</v>
-      </c>
+        <f>(V6-T6)/T6</f>
+        <v>-1.5893165521084264E-3</v>
+      </c>
+      <c r="X10" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="Y10" s="10"/>
+      <c r="Z10" s="10"/>
+      <c r="AB10" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC10" s="10"/>
+      <c r="AD10" s="10"/>
     </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>19</v>
       </c>
@@ -26731,99 +26801,129 @@
       <c r="K11" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="L11" s="5">
-        <f>(N6-L6)/L6</f>
-        <v>-0.10813911830837769</v>
-      </c>
-      <c r="M11" s="5">
-        <f>(N6-M6)/M6</f>
-        <v>-6.3706414558329879E-4</v>
-      </c>
+      <c r="L11" s="5"/>
+      <c r="M11" s="5"/>
       <c r="N11" s="5"/>
       <c r="O11" s="5">
-        <f>(N6-O6)/O6</f>
-        <v>-8.6033103483749057E-5</v>
+        <f>(O6-N6)/N6</f>
+        <v>8.6040505815489668E-5</v>
       </c>
       <c r="R11" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="S11" s="5">
-        <f>(U6-S6)/S6</f>
-        <v>-7.7684780452230276E-2</v>
-      </c>
-      <c r="T11" s="5">
-        <f>(U6-T6)/T6</f>
-        <v>-1.3240506950838436E-3</v>
-      </c>
+      <c r="S11" s="5"/>
+      <c r="T11" s="5"/>
       <c r="U11" s="5"/>
       <c r="V11" s="5">
-        <f>(U6-V6)/V6</f>
-        <v>2.6568811955068341E-4</v>
+        <f>(V6-U6)/U6</f>
+        <v>-2.6561754812380275E-4</v>
+      </c>
+      <c r="X11" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="Y11" s="5"/>
+      <c r="Z11" s="5">
+        <f>(Z8-Y8)/Y8</f>
+        <v>-5.1082025449727939E-2</v>
+      </c>
+      <c r="AB11" t="s">
+        <v>66</v>
+      </c>
+      <c r="AC11" s="5"/>
+      <c r="AD11" s="5">
+        <f>(AD8-AC8)/AC8</f>
+        <v>4.7827985156079214E-3</v>
       </c>
     </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>20</v>
       </c>
       <c r="B12">
         <v>16</v>
       </c>
-      <c r="K12" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="L12" s="5">
-        <f>(O6-L6)/L6</f>
-        <v>-0.1080623821469999</v>
-      </c>
-      <c r="M12" s="5">
-        <f>(O6-M6)/M6</f>
-        <v>-5.5107845308913195E-4</v>
-      </c>
-      <c r="N12" s="5">
-        <f>(O6-N6)/N6</f>
-        <v>8.6040505815489668E-5</v>
-      </c>
-      <c r="O12" s="4"/>
-      <c r="R12" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="S12" s="5">
-        <f>(V6-S6)/S6</f>
-        <v>-7.7929763559443824E-2</v>
-      </c>
-      <c r="T12" s="5">
-        <f>(V6-T6)/T6</f>
-        <v>-1.5893165521084264E-3</v>
-      </c>
-      <c r="U12" s="5">
-        <f>(V6-U6)/U6</f>
-        <v>-2.6561754812380275E-4</v>
-      </c>
-      <c r="V12" s="4"/>
+      <c r="K12" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="L12" s="11"/>
+      <c r="M12" s="11"/>
+      <c r="N12" s="11"/>
+      <c r="O12" s="11"/>
+      <c r="R12" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="S12" s="11"/>
+      <c r="T12" s="11"/>
+      <c r="U12" s="11"/>
+      <c r="V12" s="11"/>
+      <c r="X12" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="Y12" s="11"/>
+      <c r="Z12" s="11"/>
+      <c r="AB12" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC12" s="11"/>
+      <c r="AD12" s="11"/>
     </row>
-    <row r="13" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>21</v>
       </c>
       <c r="B13">
         <v>29</v>
       </c>
-      <c r="K13" s="10" t="s">
-        <v>59</v>
-      </c>
-      <c r="L13" s="10"/>
-      <c r="M13" s="10"/>
-      <c r="N13" s="10"/>
-      <c r="O13" s="10"/>
-      <c r="R13" s="10" t="s">
-        <v>59</v>
-      </c>
-      <c r="S13" s="10"/>
-      <c r="T13" s="10"/>
-      <c r="U13" s="10"/>
-      <c r="V13" s="10"/>
+      <c r="K13" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="L13" s="4"/>
+      <c r="M13" s="5">
+        <f>(M5-L5)/L5</f>
+        <v>-0.12697733786540796</v>
+      </c>
+      <c r="N13" s="5">
+        <f>(N5-L5)/L5</f>
+        <v>-0.1335493576210677</v>
+      </c>
+      <c r="O13" s="5">
+        <f>(O5-L5)/L5</f>
+        <v>-0.13399466428358955</v>
+      </c>
+      <c r="R13" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="S13" s="4"/>
+      <c r="T13" s="5">
+        <f>(T5-S5)/S5</f>
+        <v>-0.10249665884629357</v>
+      </c>
+      <c r="U13" s="5">
+        <f>(U5-S5)/S5</f>
+        <v>-0.11789602547880962</v>
+      </c>
+      <c r="V13" s="5">
+        <f>(V5-S5)/S5</f>
+        <v>-0.1186146728400726</v>
+      </c>
+      <c r="X13" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="Y13" s="4"/>
+      <c r="Z13" s="5">
+        <f>(Z7-Y7)/Y7</f>
+        <v>-2.0314654024011811E-2</v>
+      </c>
+      <c r="AB13" t="s">
+        <v>66</v>
+      </c>
+      <c r="AC13" s="4"/>
+      <c r="AD13" s="5">
+        <f>(AD7-AC7)/AC7</f>
+        <v>6.5433041765022584E-2</v>
+      </c>
     </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>22</v>
       </c>
@@ -26831,39 +26931,33 @@
         <v>22</v>
       </c>
       <c r="K14" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="L14" s="4"/>
-      <c r="M14" s="5">
-        <f>(L5-M5)/M5</f>
-        <v>0.14544563775119065</v>
-      </c>
+        <v>52</v>
+      </c>
+      <c r="L14" s="5"/>
+      <c r="M14" s="4"/>
       <c r="N14" s="5">
-        <f>(L5-N5)/N5</f>
-        <v>0.15413383185266477</v>
+        <f>(N5-M5)/M5</f>
+        <v>-7.5278913603350969E-3</v>
       </c>
       <c r="O14" s="5">
-        <f>(L5-O5)/O5</f>
-        <v>0.15472729642334282</v>
+        <f>(O5-M5)/M5</f>
+        <v>-8.0379659343822688E-3</v>
       </c>
       <c r="R14" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="S14" s="4"/>
-      <c r="T14" s="5">
-        <f>(S5-T5)/T5</f>
-        <v>0.11420198025618267</v>
-      </c>
+        <v>52</v>
+      </c>
+      <c r="S14" s="5"/>
+      <c r="T14" s="4"/>
       <c r="U14" s="5">
-        <f>(S5-U5)/U5</f>
-        <v>0.13365320742694087</v>
+        <f>(U5-T5)/T5</f>
+        <v>-1.7158004796640383E-2</v>
       </c>
       <c r="V14" s="5">
-        <f>(S5-V5)/V5</f>
-        <v>0.1345775442192606</v>
+        <f>(V5-T5)/T5</f>
+        <v>-1.7958723109665471E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>23</v>
       </c>
@@ -26871,125 +26965,60 @@
         <v>6</v>
       </c>
       <c r="K15" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="L15" s="5">
-        <f>(M5-L5)/L5</f>
-        <v>-0.12697733786540796</v>
-      </c>
-      <c r="M15" s="4"/>
-      <c r="N15" s="5">
-        <f>(M5-N5)/N5</f>
-        <v>7.584990343610991E-3</v>
-      </c>
+        <v>53</v>
+      </c>
+      <c r="L15" s="5"/>
+      <c r="M15" s="5"/>
+      <c r="N15" s="4"/>
       <c r="O15" s="5">
-        <f>(M5-O5)/O5</f>
-        <v>8.1030983629869074E-3</v>
+        <f>(O5-N5)/N5</f>
+        <v>-5.1394348476584161E-4</v>
       </c>
       <c r="R15" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="S15" s="5">
-        <f>(T5-S5)/S5</f>
-        <v>-0.10249665884629357</v>
-      </c>
-      <c r="T15" s="4"/>
-      <c r="U15" s="5">
-        <f>(T5-U5)/U5</f>
-        <v>1.7457541375295246E-2</v>
-      </c>
+        <v>53</v>
+      </c>
+      <c r="S15" s="5"/>
+      <c r="T15" s="5"/>
+      <c r="U15" s="4"/>
       <c r="V15" s="5">
-        <f>(T5-V5)/V5</f>
-        <v>1.82871367347535E-2</v>
-      </c>
+        <f>(V5-U5)/U5</f>
+        <v>-8.1469688610468079E-4</v>
+      </c>
+      <c r="X15" s="4"/>
+      <c r="Y15" s="5"/>
+      <c r="Z15" s="4"/>
     </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>24</v>
       </c>
       <c r="B16">
         <v>2</v>
       </c>
-      <c r="K16" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="L16" s="5">
-        <f>(N5-L5)/L5</f>
-        <v>-0.1335493576210677</v>
-      </c>
-      <c r="M16" s="5">
-        <f>(N5-M5)/M5</f>
-        <v>-7.5278913603350969E-3</v>
-      </c>
-      <c r="N16" s="4"/>
-      <c r="O16" s="5">
-        <f>(N5-O5)/O5</f>
-        <v>5.1420775849313519E-4</v>
-      </c>
-      <c r="R16" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="S16" s="5">
-        <f>(U5-S5)/S5</f>
-        <v>-0.11789602547880962</v>
-      </c>
-      <c r="T16" s="5">
-        <f>(U5-T5)/T5</f>
-        <v>-1.7158004796640383E-2</v>
-      </c>
+      <c r="K16" s="4"/>
+      <c r="L16" s="5"/>
+      <c r="M16" s="5"/>
+      <c r="N16" s="5"/>
+      <c r="O16" s="4"/>
+      <c r="S16" s="5"/>
+      <c r="T16" s="5"/>
       <c r="U16" s="4"/>
-      <c r="V16" s="5">
-        <f>(U5-V5)/V5</f>
-        <v>8.1536115830139956E-4</v>
-      </c>
+      <c r="V16" s="5"/>
     </row>
-    <row r="17" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>25</v>
       </c>
       <c r="B17">
         <v>38</v>
       </c>
-      <c r="K17" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="L17" s="5">
-        <f>(O5-L5)/L5</f>
-        <v>-0.13399466428358955</v>
-      </c>
-      <c r="M17" s="5">
-        <f>(O5-M5)/M5</f>
-        <v>-8.0379659343822688E-3</v>
-      </c>
-      <c r="N17" s="5">
-        <f>(O5-N5)/N5</f>
-        <v>-5.1394348476584161E-4</v>
-      </c>
-      <c r="O17" s="4"/>
-      <c r="R17" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="S17" s="5">
-        <f>(V5-S5)/S5</f>
-        <v>-0.1186146728400726</v>
-      </c>
-      <c r="T17" s="5">
-        <f>(V5-T5)/T5</f>
-        <v>-1.7958723109665471E-2</v>
-      </c>
-      <c r="U17" s="5">
-        <f>(V5-U5)/U5</f>
-        <v>-8.1469688610468079E-4</v>
-      </c>
+      <c r="R17" s="4"/>
+      <c r="S17" s="5"/>
+      <c r="T17" s="5"/>
+      <c r="U17" s="5"/>
       <c r="V17" s="4"/>
-      <c r="Y17" t="s">
-        <v>74</v>
-      </c>
-      <c r="Z17" t="s">
-        <v>75</v>
-      </c>
     </row>
-    <row r="18" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>26</v>
       </c>
@@ -27004,17 +27033,8 @@
       <c r="T18" s="2"/>
       <c r="U18" s="2"/>
       <c r="V18" s="2"/>
-      <c r="X18" t="s">
-        <v>55</v>
-      </c>
-      <c r="Y18" s="2">
-        <v>3.2121460000000002</v>
-      </c>
-      <c r="Z18" s="2">
-        <v>2.1843254999999999</v>
-      </c>
     </row>
-    <row r="19" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>27</v>
       </c>
@@ -27026,17 +27046,8 @@
       </c>
       <c r="U19" s="3"/>
       <c r="V19" s="3"/>
-      <c r="X19" t="s">
-        <v>56</v>
-      </c>
-      <c r="Y19" s="2">
-        <v>13.009081999999999</v>
-      </c>
-      <c r="Z19" s="2">
-        <v>12.744807</v>
-      </c>
     </row>
-    <row r="20" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>28</v>
       </c>
@@ -27067,17 +27078,20 @@
       <c r="V20" t="s">
         <v>54</v>
       </c>
-      <c r="X20" t="s">
-        <v>57</v>
-      </c>
-      <c r="Y20" s="2">
-        <v>16.492356999999998</v>
-      </c>
-      <c r="Z20" s="2">
-        <v>15.649894</v>
+      <c r="Y20" t="s">
+        <v>66</v>
+      </c>
+      <c r="Z20" t="s">
+        <v>67</v>
+      </c>
+      <c r="AA20" t="s">
+        <v>78</v>
+      </c>
+      <c r="AB20" t="s">
+        <v>79</v>
       </c>
     </row>
-    <row r="21" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>29</v>
       </c>
@@ -27112,18 +27126,22 @@
         <v>9.1399999999999995E-2</v>
       </c>
       <c r="X21" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="Y21" s="2">
-        <f>Y20-Y19</f>
-        <v>3.483274999999999</v>
+        <v>1.840646</v>
       </c>
       <c r="Z21" s="2">
-        <f>Z20-Z19</f>
-        <v>2.905087</v>
+        <v>2.1649449999999999</v>
+      </c>
+      <c r="AA21" s="2">
+        <v>5.1535289999999998</v>
+      </c>
+      <c r="AB21" s="2">
+        <v>2.4009550000000002</v>
       </c>
     </row>
-    <row r="22" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>30</v>
       </c>
@@ -27160,13 +27178,23 @@
       <c r="V22" s="2">
         <v>2.4009550000000002</v>
       </c>
-      <c r="X22" s="11" t="s">
-        <v>58</v>
-      </c>
-      <c r="Y22" s="11"/>
-      <c r="Z22" s="11"/>
+      <c r="X22" t="s">
+        <v>56</v>
+      </c>
+      <c r="Y22" s="2">
+        <v>11.962090999999999</v>
+      </c>
+      <c r="Z22" s="2">
+        <v>12.036384</v>
+      </c>
+      <c r="AA22" s="2">
+        <v>12.228700999999999</v>
+      </c>
+      <c r="AB22" s="2">
+        <v>12.142946999999999</v>
+      </c>
     </row>
-    <row r="23" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>31</v>
       </c>
@@ -27203,16 +27231,23 @@
       <c r="V23" s="2">
         <v>12.142946999999999</v>
       </c>
-      <c r="X23" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="Y23" s="5"/>
-      <c r="Z23" s="5">
-        <f>(Y20-Z20)/Z20</f>
-        <v>5.3831866209445169E-2</v>
+      <c r="X23" t="s">
+        <v>57</v>
+      </c>
+      <c r="Y23" s="2">
+        <v>15.5754</v>
+      </c>
+      <c r="Z23" s="2">
+        <v>15.774134</v>
+      </c>
+      <c r="AA23" s="2">
+        <v>16.921008</v>
+      </c>
+      <c r="AB23" s="2">
+        <v>15.732476999999999</v>
       </c>
     </row>
-    <row r="24" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>32</v>
       </c>
@@ -27253,29 +27288,40 @@
       <c r="V24" s="2">
         <v>15.732476999999999</v>
       </c>
-      <c r="X24" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="Y24" s="5">
-        <f>(Z20-Y20)/Y20</f>
-        <v>-5.1082025449727939E-2</v>
-      </c>
-      <c r="Z24" s="5"/>
+      <c r="X24" t="s">
+        <v>60</v>
+      </c>
+      <c r="Y24" s="2">
+        <f>Y23-Y22</f>
+        <v>3.613309000000001</v>
+      </c>
+      <c r="Z24" s="2">
+        <f>Z23-Z22</f>
+        <v>3.7377500000000001</v>
+      </c>
+      <c r="AA24" s="2">
+        <f>AA23-AA22</f>
+        <v>4.6923070000000013</v>
+      </c>
+      <c r="AB24" s="2">
+        <f>AB23-AB22</f>
+        <v>3.5895299999999999</v>
+      </c>
     </row>
-    <row r="25" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>33</v>
       </c>
       <c r="B25">
         <v>16</v>
       </c>
-      <c r="K25" s="11" t="s">
+      <c r="K25" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="L25" s="11"/>
-      <c r="M25" s="11"/>
-      <c r="N25" s="11"/>
-      <c r="O25" s="11"/>
+      <c r="L25" s="10"/>
+      <c r="M25" s="10"/>
+      <c r="N25" s="10"/>
+      <c r="O25" s="10"/>
       <c r="R25" t="s">
         <v>60</v>
       </c>
@@ -27296,12 +27342,14 @@
         <v>3.5895299999999999</v>
       </c>
       <c r="X25" s="10" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="Y25" s="10"/>
       <c r="Z25" s="10"/>
+      <c r="AA25" s="10"/>
+      <c r="AB25" s="10"/>
     </row>
-    <row r="26" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>34</v>
       </c>
@@ -27313,34 +27361,42 @@
       </c>
       <c r="L26" s="5"/>
       <c r="M26" s="5">
-        <f>(L23-M23)/M23</f>
-        <v>1.1939635950889808E-2</v>
+        <f>(M23-L23)/L23</f>
+        <v>-1.1798763015810211E-2</v>
       </c>
       <c r="N26" s="5">
-        <f>(L23-N23)/N23</f>
-        <v>3.3911691312952801E-3</v>
+        <f>(N23-L23)/L23</f>
+        <v>-3.3797079699547771E-3</v>
       </c>
       <c r="O26" s="5">
-        <f>(L23-O23)/O23</f>
-        <v>-1.6294443460130585E-2</v>
-      </c>
-      <c r="R26" s="11" t="s">
+        <f>(O23-L23)/L23</f>
+        <v>1.656435033003717E-2</v>
+      </c>
+      <c r="R26" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="S26" s="11"/>
-      <c r="T26" s="11"/>
-      <c r="U26" s="11"/>
-      <c r="V26" s="11"/>
-      <c r="X26" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="Y26" s="4"/>
+      <c r="S26" s="10"/>
+      <c r="T26" s="10"/>
+      <c r="U26" s="10"/>
+      <c r="V26" s="10"/>
+      <c r="X26" t="s">
+        <v>66</v>
+      </c>
+      <c r="Y26" s="5"/>
       <c r="Z26" s="5">
-        <f>(Y19-Z19)/Z19</f>
-        <v>2.0735896589097004E-2</v>
+        <f>(Z23-Y23)/Y23</f>
+        <v>1.2759479692335348E-2</v>
+      </c>
+      <c r="AA26" s="5">
+        <f>(AA23-Y23)/Y23</f>
+        <v>8.6393158442158807E-2</v>
+      </c>
+      <c r="AB26" s="5">
+        <f>(AB23-Y23)/Y23</f>
+        <v>1.0084941638737962E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>35</v>
       </c>
@@ -27350,48 +27406,47 @@
       <c r="K27" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="L27" s="5">
-        <f>(M23-L23)/L23</f>
-        <v>-1.1798763015810211E-2</v>
-      </c>
+      <c r="L27" s="5"/>
       <c r="M27" s="5"/>
       <c r="N27" s="5">
-        <f>(M23-N23)/N23</f>
-        <v>-8.4476054854416144E-3</v>
+        <f>(N23-M23)/M23</f>
+        <v>8.5195754981534505E-3</v>
       </c>
       <c r="O27" s="5">
-        <f>(M23-O23)/O23</f>
-        <v>-2.7900952199080196E-2</v>
+        <f>(O23-M23)/M23</f>
+        <v>2.8701758593630625E-2</v>
       </c>
       <c r="R27" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="S27" s="5">
-        <f>(S24-L6)/L6</f>
-        <v>-3.3115375910984304E-2</v>
-      </c>
+        <v>51</v>
+      </c>
+      <c r="S27" s="5"/>
       <c r="T27" s="5">
-        <f>(S24-M6)/M6</f>
-        <v>8.342979986894232E-2</v>
+        <f>(T24-S24)/S24</f>
+        <v>-6.4873478729201448E-2</v>
       </c>
       <c r="U27" s="5">
-        <f>(S24-N6)/N6</f>
-        <v>8.412045413976825E-2</v>
+        <f>(U24-S24)/S24</f>
+        <v>-6.2219096872884891E-2</v>
       </c>
       <c r="V27" s="5">
-        <f>(S24-O6)/O6</f>
-        <v>8.4027183892548388E-2</v>
-      </c>
-      <c r="X27" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="Y27" s="5">
-        <f>(Z19-Y19)/Y19</f>
-        <v>-2.0314654024011811E-2</v>
-      </c>
-      <c r="Z27" s="4"/>
+        <f>(V24-S24)/S24</f>
+        <v>-6.8210690056956888E-2</v>
+      </c>
+      <c r="X27" t="s">
+        <v>67</v>
+      </c>
+      <c r="Y27" s="5"/>
+      <c r="Z27" s="5"/>
+      <c r="AA27" s="5">
+        <f>(AA23-Z23)/Z23</f>
+        <v>7.2705988170253935E-2</v>
+      </c>
+      <c r="AB27" s="5">
+        <f>(AB23-Z23)/Z23</f>
+        <v>-2.6408422801531117E-3</v>
+      </c>
     </row>
-    <row r="28" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>36</v>
       </c>
@@ -27401,117 +27456,117 @@
       <c r="K28" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="L28" s="5">
-        <f>(N23-L23)/L23</f>
-        <v>-3.3797079699547771E-3</v>
-      </c>
-      <c r="M28" s="5">
-        <f>(N23-M23)/M23</f>
-        <v>8.5195754981534505E-3</v>
-      </c>
+      <c r="L28" s="5"/>
+      <c r="M28" s="5"/>
       <c r="N28" s="5"/>
       <c r="O28" s="5">
-        <f>(N23-O23)/O23</f>
-        <v>-1.9619080969657181E-2</v>
+        <f>(O23-N23)/N23</f>
+        <v>2.0011691974851635E-2</v>
       </c>
       <c r="R28" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="S28" s="5">
-        <f>($S$24-S6)/S6</f>
-        <v>-1.3043845253915689E-2</v>
-      </c>
-      <c r="T28" s="5">
-        <f>($S$24-T6)/T6</f>
-        <v>6.8668665412091767E-2</v>
-      </c>
+        <v>52</v>
+      </c>
+      <c r="S28" s="5"/>
+      <c r="T28" s="5"/>
       <c r="U28" s="5">
-        <f t="shared" ref="U28:V28" si="0">($S$24-U6)/U6</f>
-        <v>7.0085512879218659E-2</v>
+        <f>(U24-T24)/T24</f>
+        <v>2.838526975696675E-3</v>
       </c>
       <c r="V28" s="5">
-        <f t="shared" si="0"/>
-        <v>7.036982188689396E-2</v>
+        <f>(V24-T24)/T24</f>
+        <v>-3.5687270672425256E-3</v>
+      </c>
+      <c r="X28" t="s">
+        <v>78</v>
+      </c>
+      <c r="Y28" s="5"/>
+      <c r="Z28" s="5"/>
+      <c r="AA28" s="5"/>
+      <c r="AB28" s="5">
+        <f>(AB23-AA23)/AA23</f>
+        <v>-7.023996442765118E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>37</v>
       </c>
       <c r="B29">
         <v>4</v>
       </c>
-      <c r="K29" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="L29" s="5">
-        <f>(O23-L23)/L23</f>
-        <v>1.656435033003717E-2</v>
-      </c>
-      <c r="M29" s="5">
-        <f>(O23-M23)/M23</f>
-        <v>2.8701758593630625E-2</v>
-      </c>
-      <c r="N29" s="5">
-        <f>(O23-N23)/N23</f>
-        <v>2.0011691974851635E-2</v>
-      </c>
-      <c r="O29" s="4"/>
+      <c r="K29" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="L29" s="11"/>
+      <c r="M29" s="11"/>
+      <c r="N29" s="11"/>
+      <c r="O29" s="11"/>
       <c r="R29" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="S29" s="5">
-        <f>($T$24-L6)/L6</f>
-        <v>-9.5840545005415001E-2</v>
-      </c>
-      <c r="T29" s="5">
-        <f>($T$24-M6)/M6</f>
-        <v>1.3143939792561506E-2</v>
-      </c>
-      <c r="U29" s="5">
-        <f>($T$24-N6)/N6</f>
-        <v>1.3789788918239777E-2</v>
-      </c>
+        <v>53</v>
+      </c>
+      <c r="S29" s="5"/>
+      <c r="T29" s="5"/>
+      <c r="U29" s="5"/>
       <c r="V29" s="5">
-        <f>($T$24-O6)/O6</f>
-        <v>1.3702569436419006E-2</v>
-      </c>
+        <f>(V24-U24)/U24</f>
+        <v>-6.3891183581287333E-3</v>
+      </c>
+      <c r="X29" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="Y29" s="11"/>
+      <c r="Z29" s="11"/>
+      <c r="AA29" s="11"/>
+      <c r="AB29" s="11"/>
     </row>
-    <row r="30" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>38</v>
       </c>
       <c r="B30">
         <v>5</v>
       </c>
-      <c r="K30" s="10" t="s">
+      <c r="K30" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="L30" s="4"/>
+      <c r="M30" s="5">
+        <f>(M22-L22)/L22</f>
+        <v>-4.2767021493430972E-2</v>
+      </c>
+      <c r="N30" s="5">
+        <f>(N22-L22)/L22</f>
+        <v>-9.330060366791823E-2</v>
+      </c>
+      <c r="O30" s="5">
+        <f>(O22-L22)/L22</f>
+        <v>-9.1881464673040827E-2</v>
+      </c>
+      <c r="R30" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="L30" s="10"/>
-      <c r="M30" s="10"/>
-      <c r="N30" s="10"/>
-      <c r="O30" s="10"/>
-      <c r="R30" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="S30" s="5">
-        <f>($T$24-S6)/S6</f>
-        <v>-7.707112436549024E-2</v>
-      </c>
-      <c r="T30" s="5">
-        <f>($T$24-T6)/T6</f>
-        <v>-6.5958852208365952E-4</v>
-      </c>
-      <c r="U30" s="5">
-        <f t="shared" ref="U30:V30" si="1">($T$24-U6)/U6</f>
-        <v>6.6534312102204242E-4</v>
-      </c>
-      <c r="V30" s="5">
-        <f t="shared" si="1"/>
-        <v>9.3120801433540623E-4</v>
+      <c r="S30" s="11"/>
+      <c r="T30" s="11"/>
+      <c r="U30" s="11"/>
+      <c r="V30" s="11"/>
+      <c r="X30" t="s">
+        <v>66</v>
+      </c>
+      <c r="Y30" s="4"/>
+      <c r="Z30" s="5">
+        <f>(Z22-Y22)/Y22</f>
+        <v>6.2107034631320593E-3</v>
+      </c>
+      <c r="AA30" s="5">
+        <f>(AA22-Y22)/Y22</f>
+        <v>2.2287909363003511E-2</v>
+      </c>
+      <c r="AB30" s="5">
+        <f>(AB22-Y22)/Y22</f>
+        <v>1.5119095816943741E-2</v>
       </c>
     </row>
-    <row r="31" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>39</v>
       </c>
@@ -27519,42 +27574,49 @@
         <v>6</v>
       </c>
       <c r="K31" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="L31" s="5"/>
+      <c r="M31" s="4"/>
+      <c r="N31" s="5">
+        <f>(N22-M22)/M22</f>
+        <v>-5.2791309231037385E-2</v>
+      </c>
+      <c r="O31" s="5">
+        <f>(O22-M22)/M22</f>
+        <v>-5.1308766290350714E-2</v>
+      </c>
+      <c r="R31" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="L31" s="4"/>
-      <c r="M31" s="5">
-        <f>(L22-M22)/M22</f>
-        <v>4.4677756046552136E-2</v>
-      </c>
-      <c r="N31" s="5">
-        <f>(L22-N22)/N22</f>
-        <v>0.10290136294934353</v>
-      </c>
-      <c r="O31" s="5">
-        <f>(L22-O22)/O22</f>
-        <v>0.10117783207669008</v>
-      </c>
-      <c r="R31" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="S31" s="5">
-        <f>($U$24-L6)/L6</f>
-        <v>-9.3274064002081658E-2</v>
-      </c>
+      <c r="S31" s="4"/>
       <c r="T31" s="5">
-        <f>($U$24-M6)/M6</f>
-        <v>1.6019776195926299E-2</v>
+        <f>(T23-S23)/S23</f>
+        <v>-9.8873663230320444E-2</v>
       </c>
       <c r="U31" s="5">
-        <f t="shared" ref="U31:V31" si="2">($U$24-N6)/N6</f>
-        <v>1.6667458581770038E-2</v>
+        <f>(U23-S23)/S23</f>
+        <v>-9.3618004245734146E-2</v>
       </c>
       <c r="V31" s="5">
-        <f t="shared" si="2"/>
-        <v>1.6579991525097312E-2</v>
+        <f>(V23-S23)/S23</f>
+        <v>-0.1058357011768367</v>
+      </c>
+      <c r="X31" t="s">
+        <v>67</v>
+      </c>
+      <c r="Y31" s="5"/>
+      <c r="Z31" s="4"/>
+      <c r="AA31" s="5">
+        <f>(AA22-Z22)/Z22</f>
+        <v>1.5977971457208345E-2</v>
+      </c>
+      <c r="AB31" s="5">
+        <f>(AB22-Z22)/Z22</f>
+        <v>8.8534064715781353E-3</v>
       </c>
     </row>
-    <row r="32" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>40</v>
       </c>
@@ -27562,39 +27624,37 @@
         <v>1</v>
       </c>
       <c r="K32" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="L32" s="5"/>
+      <c r="M32" s="5"/>
+      <c r="N32" s="4"/>
+      <c r="O32" s="5">
+        <f>(O22-N22)/N22</f>
+        <v>1.5651703316648397E-3</v>
+      </c>
+      <c r="R32" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="L32" s="5">
-        <f>(M22-L22)/L22</f>
-        <v>-4.2767021493430972E-2</v>
-      </c>
-      <c r="M32" s="4"/>
-      <c r="N32" s="5">
-        <f>(M22-N22)/N22</f>
-        <v>5.5733556654954643E-2</v>
-      </c>
-      <c r="O32" s="5">
-        <f>(M22-O22)/O22</f>
-        <v>5.408373606417656E-2</v>
-      </c>
-      <c r="R32" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="S32" s="5">
-        <f>($U$24-S6)/S6</f>
-        <v>-7.4451365855352281E-2</v>
-      </c>
-      <c r="T32" s="5">
-        <f>($U$24-T6)/T6</f>
-        <v>2.1770661938002212E-3</v>
-      </c>
+      <c r="S32" s="5"/>
+      <c r="T32" s="4"/>
       <c r="U32" s="5">
-        <f>($U$24-U6)/U6</f>
-        <v>3.5057586911158328E-3</v>
+        <f>(U23-T23)/T23</f>
+        <v>5.8323220287030573E-3</v>
       </c>
       <c r="V32" s="5">
-        <f>($U$24-V6)/V6</f>
-        <v>3.7723782491007572E-3</v>
+        <f>(V23-T23)/T23</f>
+        <v>-7.725928831992069E-3</v>
+      </c>
+      <c r="X32" t="s">
+        <v>78</v>
+      </c>
+      <c r="Y32" s="5"/>
+      <c r="Z32" s="5"/>
+      <c r="AA32" s="4"/>
+      <c r="AB32" s="5">
+        <f>(AB22-AA22)/AA22</f>
+        <v>-7.0125191547327614E-3</v>
       </c>
     </row>
     <row r="33" spans="1:22" x14ac:dyDescent="0.25">
@@ -27604,40 +27664,15 @@
       <c r="B33">
         <v>28</v>
       </c>
-      <c r="K33" s="4" t="s">
+      <c r="R33" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="L33" s="5">
-        <f>(N22-L22)/L22</f>
-        <v>-9.330060366791823E-2</v>
-      </c>
-      <c r="M33" s="5">
-        <f>(N22-M22)/M22</f>
-        <v>-5.2791309231037385E-2</v>
-      </c>
-      <c r="N33" s="4"/>
-      <c r="O33" s="5">
-        <f>(N22-O22)/O22</f>
-        <v>-1.5627244017945823E-3</v>
-      </c>
-      <c r="R33" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="S33" s="5">
-        <f>($V$24-L6)/L6</f>
-        <v>-9.9067243325557428E-2</v>
-      </c>
-      <c r="T33" s="5">
-        <f t="shared" ref="T33:V33" si="3">($V$24-M6)/M6</f>
-        <v>9.5283055916110596E-3</v>
-      </c>
-      <c r="U33" s="5">
-        <f t="shared" si="3"/>
-        <v>1.0171849858033167E-2</v>
-      </c>
+      <c r="S33" s="5"/>
+      <c r="T33" s="5"/>
+      <c r="U33" s="4"/>
       <c r="V33" s="5">
-        <f t="shared" si="3"/>
-        <v>1.0084941638737962E-2</v>
+        <f>(V23-U23)/U23</f>
+        <v>-1.3479633298469624E-2</v>
       </c>
     </row>
     <row r="34" spans="1:22" x14ac:dyDescent="0.25">
@@ -27647,41 +27682,16 @@
       <c r="B34">
         <v>0</v>
       </c>
-      <c r="K34" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="L34" s="5">
-        <f>(O22-L22)/L22</f>
-        <v>-9.1881464673040827E-2</v>
-      </c>
-      <c r="M34" s="5">
-        <f>(O22-M22)/M22</f>
-        <v>-5.1308766290350714E-2</v>
-      </c>
-      <c r="N34" s="5">
-        <f>(O22-N22)/N22</f>
-        <v>1.5651703316648397E-3</v>
-      </c>
+      <c r="K34" s="4"/>
+      <c r="L34" s="5"/>
+      <c r="M34" s="5"/>
+      <c r="N34" s="5"/>
       <c r="O34" s="4"/>
-      <c r="R34" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="S34" s="5">
-        <f>($V$24-S6)/S6</f>
-        <v>-8.0364805625106825E-2</v>
-      </c>
-      <c r="T34" s="5">
-        <f t="shared" ref="T34:V34" si="4">($V$24-T6)/T6</f>
-        <v>-4.2259616979141825E-3</v>
-      </c>
-      <c r="U34" s="5">
-        <f t="shared" si="4"/>
-        <v>-2.9057583742254783E-3</v>
-      </c>
-      <c r="V34" s="5">
-        <f t="shared" si="4"/>
-        <v>-2.6408422801531117E-3</v>
-      </c>
+      <c r="R34" s="4"/>
+      <c r="S34" s="5"/>
+      <c r="T34" s="5"/>
+      <c r="U34" s="5"/>
+      <c r="V34" s="5"/>
     </row>
     <row r="35" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
@@ -27690,13 +27700,6 @@
       <c r="B35">
         <v>0</v>
       </c>
-      <c r="R35" s="10" t="s">
-        <v>59</v>
-      </c>
-      <c r="S35" s="10"/>
-      <c r="T35" s="10"/>
-      <c r="U35" s="10"/>
-      <c r="V35" s="10"/>
     </row>
     <row r="36" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
@@ -27705,25 +27708,11 @@
       <c r="B36">
         <v>41</v>
       </c>
-      <c r="R36" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="S36" s="5">
-        <f>($S$23-L5)/L5</f>
-        <v>-1.6848967776839655E-2</v>
-      </c>
-      <c r="T36" s="5">
-        <f t="shared" ref="T36:V36" si="5">($S$23-M5)/M5</f>
-        <v>0.12614606111059928</v>
-      </c>
-      <c r="U36" s="5">
-        <f t="shared" si="5"/>
-        <v>0.13468786810961875</v>
-      </c>
-      <c r="V36" s="5">
-        <f t="shared" si="5"/>
-        <v>0.13527133341486874</v>
-      </c>
+      <c r="R36" s="4"/>
+      <c r="S36" s="5"/>
+      <c r="T36" s="5"/>
+      <c r="U36" s="5"/>
+      <c r="V36" s="5"/>
     </row>
     <row r="37" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
@@ -27732,181 +27721,87 @@
       <c r="B37">
         <v>60</v>
       </c>
-      <c r="R37" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="S37" s="5">
-        <f>($S$23-S5)/S5</f>
-        <v>-5.5646474706638003E-3</v>
-      </c>
-      <c r="T37" s="5">
-        <f t="shared" ref="T37:V37" si="6">($S$23-T5)/T5</f>
-        <v>0.10800183902494151</v>
-      </c>
-      <c r="U37" s="5">
-        <f t="shared" si="6"/>
-        <v>0.12734482697362265</v>
-      </c>
-      <c r="V37" s="5">
-        <f t="shared" si="6"/>
-        <v>0.12826402015754895</v>
-      </c>
+      <c r="R37" s="4"/>
+      <c r="S37" s="5"/>
+      <c r="T37" s="5"/>
+      <c r="U37" s="5"/>
+      <c r="V37" s="5"/>
     </row>
     <row r="38" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>46</v>
       </c>
-      <c r="R38" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="S38" s="5">
-        <f>($T$23-L5)/L5</f>
-        <v>-0.11405671184141433</v>
-      </c>
-      <c r="T38" s="5">
-        <f t="shared" ref="T38:V38" si="7">($T$23-M5)/M5</f>
-        <v>1.4799874716198029E-2</v>
-      </c>
-      <c r="U38" s="5">
-        <f t="shared" si="7"/>
-        <v>2.2497121966618034E-2</v>
-      </c>
-      <c r="V38" s="5">
-        <f t="shared" si="7"/>
-        <v>2.3022897919770174E-2</v>
-      </c>
+      <c r="R38" s="4"/>
+      <c r="S38" s="5"/>
+      <c r="T38" s="5"/>
+      <c r="U38" s="5"/>
+      <c r="V38" s="5"/>
     </row>
     <row r="39" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>47</v>
       </c>
-      <c r="R39" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="S39" s="5">
-        <f>($T$23-S5)/S5</f>
-        <v>-0.10388811362097437</v>
-      </c>
-      <c r="T39" s="5">
-        <f t="shared" ref="T39:V39" si="8">($T$23-T5)/T5</f>
-        <v>-1.5503616653862815E-3</v>
-      </c>
-      <c r="U39" s="5">
-        <f t="shared" si="8"/>
-        <v>1.5880114206988812E-2</v>
-      </c>
-      <c r="V39" s="5">
-        <f t="shared" si="8"/>
-        <v>1.6708423393603979E-2</v>
-      </c>
+      <c r="R39" s="4"/>
+      <c r="S39" s="5"/>
+      <c r="T39" s="5"/>
+      <c r="U39" s="5"/>
+      <c r="V39" s="5"/>
     </row>
     <row r="40" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>48</v>
       </c>
-      <c r="R40" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="S40" s="5">
-        <f>($U$23-L5)/L5</f>
-        <v>-0.10888960528570539</v>
-      </c>
-      <c r="T40" s="5">
-        <f>($U$23-M5)/M5</f>
-        <v>2.0718514380230414E-2</v>
-      </c>
-      <c r="U40" s="5">
-        <f t="shared" ref="U40:V40" si="9">($U$23-N5)/N5</f>
-        <v>2.846065445534942E-2</v>
-      </c>
-      <c r="V40" s="5">
-        <f t="shared" si="9"/>
-        <v>2.8989496903175288E-2</v>
-      </c>
+      <c r="R40" s="4"/>
+      <c r="S40" s="5"/>
+      <c r="T40" s="5"/>
+      <c r="U40" s="5"/>
+      <c r="V40" s="5"/>
     </row>
     <row r="41" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>49</v>
       </c>
-      <c r="R41" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="S41" s="5">
-        <f>($U$23-S5)/S5</f>
-        <v>-9.866170052586333E-2</v>
-      </c>
-      <c r="T41" s="5">
-        <f t="shared" ref="T41:V41" si="10">($U$23-T5)/T5</f>
-        <v>4.2729181548232867E-3</v>
-      </c>
-      <c r="U41" s="5">
-        <f t="shared" si="10"/>
-        <v>2.1805054175599609E-2</v>
-      </c>
-      <c r="V41" s="5">
-        <f t="shared" si="10"/>
-        <v>2.263819432813045E-2</v>
-      </c>
+      <c r="R41" s="4"/>
+      <c r="S41" s="5"/>
+      <c r="T41" s="5"/>
+      <c r="U41" s="5"/>
+      <c r="V41" s="5"/>
     </row>
     <row r="42" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>50</v>
       </c>
-      <c r="R42" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="S42" s="5">
-        <f>($V$23-L5)/L5</f>
-        <v>-0.12090144663490861</v>
-      </c>
-      <c r="T42" s="5">
-        <f t="shared" ref="T42:V42" si="11">($V$23-M5)/M5</f>
-        <v>6.9596031054262155E-3</v>
-      </c>
-      <c r="U42" s="5">
-        <f t="shared" si="11"/>
-        <v>1.4597381971387231E-2</v>
-      </c>
-      <c r="V42" s="5">
-        <f t="shared" si="11"/>
-        <v>1.5119095816943741E-2</v>
-      </c>
+      <c r="R42" s="4"/>
+      <c r="S42" s="5"/>
+      <c r="T42" s="5"/>
+      <c r="U42" s="5"/>
+      <c r="V42" s="5"/>
     </row>
     <row r="43" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="R43" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="S43" s="5">
-        <f>($V$23-S5)/S5</f>
-        <v>-0.11081141028064088</v>
-      </c>
-      <c r="T43" s="5">
-        <f t="shared" ref="T43:V43" si="12">($V$23-T5)/T5</f>
-        <v>-9.2643125134877283E-3</v>
-      </c>
-      <c r="U43" s="5">
-        <f t="shared" si="12"/>
-        <v>8.0314967427896414E-3</v>
-      </c>
-      <c r="V43" s="5">
-        <f t="shared" si="12"/>
-        <v>8.8534064715781353E-3</v>
-      </c>
+      <c r="R43" s="4"/>
+      <c r="S43" s="5"/>
+      <c r="T43" s="5"/>
+      <c r="U43" s="5"/>
+      <c r="V43" s="5"/>
     </row>
     <row r="62" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="65" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <mergeCells count="10">
-    <mergeCell ref="X22:Z22"/>
-    <mergeCell ref="X25:Z25"/>
-    <mergeCell ref="R35:V35"/>
+  <mergeCells count="14">
+    <mergeCell ref="X10:Z10"/>
+    <mergeCell ref="X12:Z12"/>
+    <mergeCell ref="R30:V30"/>
     <mergeCell ref="K25:O25"/>
     <mergeCell ref="K8:O8"/>
     <mergeCell ref="R8:V8"/>
-    <mergeCell ref="K13:O13"/>
-    <mergeCell ref="R13:V13"/>
-    <mergeCell ref="K30:O30"/>
+    <mergeCell ref="K12:O12"/>
+    <mergeCell ref="R12:V12"/>
+    <mergeCell ref="K29:O29"/>
     <mergeCell ref="R26:V26"/>
+    <mergeCell ref="X25:AB25"/>
+    <mergeCell ref="X29:AB29"/>
+    <mergeCell ref="AB10:AD10"/>
+    <mergeCell ref="AB12:AD12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -29157,13 +29052,13 @@
       <c r="J36">
         <v>28.283641966836871</v>
       </c>
-      <c r="L36" s="11" t="s">
+      <c r="L36" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="M36" s="11"/>
-      <c r="N36" s="11"/>
-      <c r="O36" s="11"/>
-      <c r="P36" s="11"/>
+      <c r="M36" s="10"/>
+      <c r="N36" s="10"/>
+      <c r="O36" s="10"/>
+      <c r="P36" s="10"/>
     </row>
     <row r="37" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
@@ -29316,13 +29211,13 @@
       <c r="F41">
         <v>18.391079999999999</v>
       </c>
-      <c r="L41" s="10" t="s">
+      <c r="L41" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="M41" s="10"/>
-      <c r="N41" s="10"/>
-      <c r="O41" s="10"/>
-      <c r="P41" s="10"/>
+      <c r="M41" s="11"/>
+      <c r="N41" s="11"/>
+      <c r="O41" s="11"/>
+      <c r="P41" s="11"/>
     </row>
     <row r="42" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C42">
@@ -30492,13 +30387,13 @@
       <c r="I34">
         <v>-14.94128081710544</v>
       </c>
-      <c r="K34" s="11" t="s">
+      <c r="K34" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="L34" s="11"/>
-      <c r="M34" s="11"/>
-      <c r="N34" s="11"/>
-      <c r="O34" s="11"/>
+      <c r="L34" s="10"/>
+      <c r="M34" s="10"/>
+      <c r="N34" s="10"/>
+      <c r="O34" s="10"/>
     </row>
     <row r="35" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A35">
@@ -30678,13 +30573,13 @@
       <c r="E39">
         <v>18.380500000000001</v>
       </c>
-      <c r="K39" s="10" t="s">
+      <c r="K39" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="L39" s="10"/>
-      <c r="M39" s="10"/>
-      <c r="N39" s="10"/>
-      <c r="O39" s="10"/>
+      <c r="L39" s="11"/>
+      <c r="M39" s="11"/>
+      <c r="N39" s="11"/>
+      <c r="O39" s="11"/>
     </row>
     <row r="40" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B40">
@@ -31885,13 +31780,13 @@
       <c r="J31">
         <v>-2.1059569045901299</v>
       </c>
-      <c r="M31" s="11" t="s">
+      <c r="M31" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="N31" s="11"/>
-      <c r="O31" s="11"/>
-      <c r="P31" s="11"/>
-      <c r="Q31" s="11"/>
+      <c r="N31" s="10"/>
+      <c r="O31" s="10"/>
+      <c r="P31" s="10"/>
+      <c r="Q31" s="10"/>
     </row>
     <row r="32" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
@@ -32119,13 +32014,13 @@
       <c r="J36">
         <v>36.996688846731558</v>
       </c>
-      <c r="M36" s="10" t="s">
+      <c r="M36" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="N36" s="10"/>
-      <c r="O36" s="10"/>
-      <c r="P36" s="10"/>
-      <c r="Q36" s="10"/>
+      <c r="N36" s="11"/>
+      <c r="O36" s="11"/>
+      <c r="P36" s="11"/>
+      <c r="Q36" s="11"/>
     </row>
     <row r="37" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
@@ -32243,7 +32138,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="P32" sqref="P32"/>
     </sheetView>
   </sheetViews>
@@ -33462,13 +33357,13 @@
       <c r="J35">
         <v>-9.2707664974478199</v>
       </c>
-      <c r="L35" s="11" t="s">
+      <c r="L35" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="M35" s="11"/>
-      <c r="N35" s="11"/>
-      <c r="O35" s="11"/>
-      <c r="P35" s="11"/>
+      <c r="M35" s="10"/>
+      <c r="N35" s="10"/>
+      <c r="O35" s="10"/>
+      <c r="P35" s="10"/>
     </row>
     <row r="36" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
@@ -33639,13 +33534,13 @@
       <c r="F40">
         <v>21.985949999999999</v>
       </c>
-      <c r="L40" s="10" t="s">
+      <c r="L40" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="M40" s="10"/>
-      <c r="N40" s="10"/>
-      <c r="O40" s="10"/>
-      <c r="P40" s="10"/>
+      <c r="M40" s="11"/>
+      <c r="N40" s="11"/>
+      <c r="O40" s="11"/>
+      <c r="P40" s="11"/>
     </row>
     <row r="41" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C41">
@@ -36022,10 +35917,10 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="D1" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -36318,10 +36213,10 @@
         <v>19.72054</v>
       </c>
       <c r="I23" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="J23" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
@@ -36431,11 +36326,11 @@
       <c r="D28" s="2">
         <v>19.757439999999999</v>
       </c>
-      <c r="H28" s="11" t="s">
+      <c r="H28" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="I28" s="11"/>
-      <c r="J28" s="11"/>
+      <c r="I28" s="10"/>
+      <c r="J28" s="10"/>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
@@ -36451,7 +36346,7 @@
         <v>19.692799999999998</v>
       </c>
       <c r="H29" s="4" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="I29" s="5"/>
       <c r="J29" s="5">
@@ -36473,7 +36368,7 @@
         <v>19.007960000000001</v>
       </c>
       <c r="H30" s="4" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="I30" s="5">
         <f>(J26-I26)/I26</f>
@@ -36494,11 +36389,11 @@
       <c r="D31" s="2">
         <v>18.879629999999999</v>
       </c>
-      <c r="H31" s="10" t="s">
+      <c r="H31" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="I31" s="10"/>
-      <c r="J31" s="10"/>
+      <c r="I31" s="11"/>
+      <c r="J31" s="11"/>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
@@ -36514,7 +36409,7 @@
         <v>18.349519999999998</v>
       </c>
       <c r="H32" s="4" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="I32" s="4"/>
       <c r="J32" s="5">
@@ -36536,7 +36431,7 @@
         <v>18.206040000000002</v>
       </c>
       <c r="H33" s="4" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="I33" s="5">
         <f>(J25-I25)/I25</f>
@@ -36700,28 +36595,28 @@
         <v>1</v>
       </c>
       <c r="C1" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="G1" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="H1" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="I1" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="J1" s="9" t="s">
         <v>77</v>
-      </c>
-      <c r="E1" s="9" t="s">
-        <v>78</v>
-      </c>
-      <c r="F1" s="9" t="s">
-        <v>79</v>
-      </c>
-      <c r="G1" s="9" t="s">
-        <v>80</v>
-      </c>
-      <c r="H1" s="9" t="s">
-        <v>81</v>
-      </c>
-      <c r="I1" s="9" t="s">
-        <v>82</v>
-      </c>
-      <c r="J1" s="9" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">

</xml_diff>